<commit_message>
probando cambios en homeinmo
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\public_html\assets\ddbb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A446283E-E88B-48EA-AFF7-02FE1ECF1672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7905"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
   <si>
     <t>id</t>
   </si>
@@ -584,11 +585,51 @@
   <si>
     <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m16!1m12!1m3!1d777.7260877556857!2d-60.32582248619418!3d-38.8923687918754!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!2m1!1s15%20y%2022%20reta%20tres%20arroyos!5e1!3m2!1ses-419!2sar!4v1740171744008!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
   </si>
+  <si>
+    <t>img1:las_acacias_U5_1-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img2:las_acacias_U5_1-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img3:las_acacias_U5_1-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img4:las_acacias_U5_1-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img5:las_acacias_U5_10-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img6:las_acacias_U5_10-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img7:las_acacias_U5_10-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img8:las_acacias_U5_10-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img9:las_acacias_U5_11-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img10:las_acacias_U5_11-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img11:las_acacias_U5_11-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img12:las_acacias_U5_11-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img13:las_acacias_U5_12-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img14:las_acacias_U5_12-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img15:las_acacias_U5_12-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img16:las_acacias_U5_12-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img17:las_acacias_U5_2-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img18:las_acacias_U5_2-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img19:las_acacias_U5_2-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img20:las_acacias_U5_2-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img21:las_acacias_U5_3-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img22:las_acacias_U5_3-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img23:las_acacias_U5_3-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img24:las_acacias_U5_3-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img25:las_acacias_U5_4-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img26:las_acacias_U5_4-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img27:las_acacias_U5_4-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img28:las_acacias_U5_4-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img29:las_acacias_U5_5-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img30:las_acacias_U5_5-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img31:las_acacias_U5_5-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img32:las_acacias_U5_5-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img33:las_acacias_U5_6-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img34:las_acacias_U5_6-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img35:las_acacias_U5_6-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img36:las_acacias_U5_6-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img37:las_acacias_U5_7-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img38:las_acacias_U5_7-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img39:las_acacias_U5_7-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img40:las_acacias_U5_7-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img41:las_acacias_U5_8-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img42:las_acacias_U5_8-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img43:las_acacias_U5_8-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img44:las_acacias_U5_8-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img45:las_acacias_U5_9-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img46:las_acacias_U5_9-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img47:las_acacias_U5_9-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img48:las_acacias_U5_9-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img49:las_acacias_U5_1-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img50:las_acacias_U5_1-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img51:las_acacias_U5_1-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img52:las_acacias_U5_1-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img53:las_acacias_U5_10-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img54:las_acacias_U5_10-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img55:las_acacias_U5_10-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img56:las_acacias_U5_10-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img57:las_acacias_U5_11-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img58:las_acacias_U5_11-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img59:las_acacias_U5_11-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img60:las_acacias_U5_11-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img61:las_acacias_U5_12-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img62:las_acacias_U5_12-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img63:las_acacias_U5_12-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img64:las_acacias_U5_12-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img65:las_acacias_U5_2-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img66:las_acacias_U5_2-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img67:las_acacias_U5_2-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img68:las_acacias_U5_2-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img69:las_acacias_U5_3-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img70:las_acacias_U5_3-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img71:las_acacias_U5_3-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img72:las_acacias_U5_3-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img73:las_acacias_U5_4-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img74:las_acacias_U5_4-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img75:las_acacias_U5_4-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img76:las_acacias_U5_4-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img77:las_acacias_U5_5-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img78:las_acacias_U5_5-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img79:las_acacias_U5_5-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img80:las_acacias_U5_5-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img81:las_acacias_U5_6-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img82:las_acacias_U5_6-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img83:las_acacias_U5_6-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img84:las_acacias_U5_6-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img85:las_acacias_U5_7-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img86:las_acacias_U5_7-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img87:las_acacias_U5_7-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img88:las_acacias_U5_7-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img89:las_acacias_U5_8-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img90:las_acacias_U5_8-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img91:las_acacias_U5_8-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img92:las_acacias_U5_8-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img93:las_acacias_U5_9-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img94:las_acacias_U5_9-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img95:las_acacias_U5_9-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img96:las_acacias_U5_9-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;</t>
+  </si>
+  <si>
+    <t>casa-venta-las-acacias</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/el pato/las_acacias_U5</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1574.699881346684!2d-58.175552709271074!3d-34.88028292737519!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2d9ac6824eb15%3A0x65a407b05300e937!2sBarrio%20Las%20Acacias!5e0!3m2!1ses-419!2sar!4v1746032203480!5m2!1ses-419!2sar" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>El Pato, Berazategui</t>
+  </si>
+  <si>
+    <t>Calle 517 y Autovia 2</t>
+  </si>
+  <si>
+    <t>sqrmeters:🏠 92 m2 cubiertos; bedrooms:🛏️ 3 dormitorios; bathrooms:🚽 1 baño; livingroom:🛋️ Cocina, comedor y sala de estar; garage:🚘 Cochera</t>
+  </si>
+  <si>
+    <t>Ubicada en un entorno tranquilo y organizado, esta propiedad cuenta con todo lo necesario para mudarse ya. Ideal para familias que buscan seguridad, comodidad y una excelente relación precio-calidad. Características principales:
+-3 dormitorios
+-Gran living-comedor
+-Cocina independiente
+-Hall de entrada
+-Baño completo
+-Lavadero
+-Patio trasero
+-Espacio para vehículo
+Entorno y servicios:
+-Barrio cerrado con portón eléctrico
+-Alarma vecinal
+-Cámaras de seguridad
+-Expensas muy bajas: menos de $5.000 por mes (incluyen corte de pasto de espacios comunes, uso de plaza interna y servicio de agua para el barrio)
+-Plaza interna de uso común, ideal para niños o para disfrutar al aire libre.
+Accesos rápidos a la autopista y cercanía a comercios.
+Documentación al día – lista para escriturar.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -652,7 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -940,18 +980,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="45.28515625" customWidth="1"/>
-    <col min="14" max="16" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1027,7 +1066,7 @@
       <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>90</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1061,7 +1100,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B12" si="0">CONCATENATE("/",A3,".html")</f>
+        <f t="shared" ref="B3:B13" si="0">CONCATENATE("/",A3,".html")</f>
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1104,7 +1143,7 @@
         <v>20</v>
       </c>
       <c r="P3" s="5"/>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="8" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1119,7 +1158,7 @@
       <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>79</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1156,7 +1195,7 @@
         <v>30</v>
       </c>
       <c r="P4" s="5"/>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="8" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1171,7 +1210,7 @@
       <c r="C5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1204,7 +1243,7 @@
       <c r="N5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" t="s">
         <v>65</v>
       </c>
       <c r="Q5" t="s">
@@ -1222,7 +1261,7 @@
       <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1255,10 +1294,10 @@
       <c r="N6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="7"/>
+      <c r="P6" s="6"/>
       <c r="Q6" t="s">
         <v>94</v>
       </c>
@@ -1274,7 +1313,7 @@
       <c r="C7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1307,10 +1346,10 @@
       <c r="N7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="7"/>
+      <c r="P7" s="6"/>
       <c r="Q7" t="s">
         <v>97</v>
       </c>
@@ -1326,7 +1365,7 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>83</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1359,10 +1398,10 @@
       <c r="N8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="7"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1375,7 +1414,7 @@
       <c r="C9" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1408,10 +1447,10 @@
       <c r="N9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" t="s">
         <v>56</v>
       </c>
-      <c r="P9" s="7"/>
+      <c r="P9" s="6"/>
       <c r="Q9" t="s">
         <v>93</v>
       </c>
@@ -1427,7 +1466,7 @@
       <c r="C10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>85</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1460,10 +1499,10 @@
       <c r="N10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="7"/>
+      <c r="P10" s="6"/>
       <c r="Q10" t="s">
         <v>99</v>
       </c>
@@ -1479,7 +1518,7 @@
       <c r="C11" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>86</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1512,10 +1551,10 @@
       <c r="N11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="7"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1528,7 +1567,7 @@
       <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1561,13 +1600,58 @@
       <c r="N12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" t="s">
         <v>52</v>
       </c>
-      <c r="P12" s="7"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/casa-venta-las-acacias.html</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13">
+        <v>55000</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -1592,7 +1676,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
no termine de arreglar la importacion de imagenes
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A446283E-E88B-48EA-AFF7-02FE1ECF1672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D983CB-AB4C-4227-9788-7D38874B778A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
   <si>
     <t>id</t>
   </si>
@@ -586,13 +586,7 @@
     <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m16!1m12!1m3!1d777.7260877556857!2d-60.32582248619418!3d-38.8923687918754!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!2m1!1s15%20y%2022%20reta%20tres%20arroyos!5e1!3m2!1ses-419!2sar!4v1740171744008!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
   </si>
   <si>
-    <t>img1:las_acacias_U5_1-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img2:las_acacias_U5_1-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img3:las_acacias_U5_1-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img4:las_acacias_U5_1-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img5:las_acacias_U5_10-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img6:las_acacias_U5_10-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img7:las_acacias_U5_10-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img8:las_acacias_U5_10-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img9:las_acacias_U5_11-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img10:las_acacias_U5_11-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img11:las_acacias_U5_11-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img12:las_acacias_U5_11-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img13:las_acacias_U5_12-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img14:las_acacias_U5_12-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img15:las_acacias_U5_12-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img16:las_acacias_U5_12-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img17:las_acacias_U5_2-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img18:las_acacias_U5_2-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img19:las_acacias_U5_2-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img20:las_acacias_U5_2-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img21:las_acacias_U5_3-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img22:las_acacias_U5_3-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img23:las_acacias_U5_3-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img24:las_acacias_U5_3-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img25:las_acacias_U5_4-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img26:las_acacias_U5_4-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img27:las_acacias_U5_4-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img28:las_acacias_U5_4-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img29:las_acacias_U5_5-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img30:las_acacias_U5_5-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img31:las_acacias_U5_5-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img32:las_acacias_U5_5-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img33:las_acacias_U5_6-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img34:las_acacias_U5_6-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img35:las_acacias_U5_6-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img36:las_acacias_U5_6-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img37:las_acacias_U5_7-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img38:las_acacias_U5_7-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img39:las_acacias_U5_7-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img40:las_acacias_U5_7-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img41:las_acacias_U5_8-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img42:las_acacias_U5_8-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img43:las_acacias_U5_8-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img44:las_acacias_U5_8-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img45:las_acacias_U5_9-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img46:las_acacias_U5_9-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img47:las_acacias_U5_9-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img48:las_acacias_U5_9-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img49:las_acacias_U5_1-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img50:las_acacias_U5_1-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img51:las_acacias_U5_1-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img52:las_acacias_U5_1-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img53:las_acacias_U5_10-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img54:las_acacias_U5_10-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img55:las_acacias_U5_10-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img56:las_acacias_U5_10-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img57:las_acacias_U5_11-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img58:las_acacias_U5_11-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img59:las_acacias_U5_11-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img60:las_acacias_U5_11-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img61:las_acacias_U5_12-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img62:las_acacias_U5_12-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img63:las_acacias_U5_12-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img64:las_acacias_U5_12-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img65:las_acacias_U5_2-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img66:las_acacias_U5_2-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img67:las_acacias_U5_2-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img68:las_acacias_U5_2-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img69:las_acacias_U5_3-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img70:las_acacias_U5_3-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img71:las_acacias_U5_3-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img72:las_acacias_U5_3-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img73:las_acacias_U5_4-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img74:las_acacias_U5_4-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img75:las_acacias_U5_4-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img76:las_acacias_U5_4-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img77:las_acacias_U5_5-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img78:las_acacias_U5_5-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img79:las_acacias_U5_5-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img80:las_acacias_U5_5-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img81:las_acacias_U5_6-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img82:las_acacias_U5_6-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img83:las_acacias_U5_6-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img84:las_acacias_U5_6-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img85:las_acacias_U5_7-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img86:las_acacias_U5_7-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img87:las_acacias_U5_7-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img88:las_acacias_U5_7-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img89:las_acacias_U5_8-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img90:las_acacias_U5_8-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img91:las_acacias_U5_8-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img92:las_acacias_U5_8-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img93:las_acacias_U5_9-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img94:las_acacias_U5_9-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img95:las_acacias_U5_9-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img96:las_acacias_U5_9-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;</t>
-  </si>
-  <si>
     <t>casa-venta-las-acacias</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/berazategui/el pato/las_acacias_U5</t>
   </si>
   <si>
     <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1574.699881346684!2d-58.175552709271074!3d-34.88028292737519!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2d9ac6824eb15%3A0x65a407b05300e937!2sBarrio%20Las%20Acacias!5e0!3m2!1ses-419!2sar!4v1746032203480!5m2!1ses-419!2sar" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
@@ -624,6 +618,42 @@
 -Plaza interna de uso común, ideal para niños o para disfrutar al aire libre.
 Accesos rápidos a la autopista y cercanía a comercios.
 Documentación al día – lista para escriturar.</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/sebastiangaboto/5/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/florenciovarela/laflorida</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/aromas/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/elangel/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/nuevohorizonte/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/santateresita</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/tresarroyos/cabanareta/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/sanluis/corderas/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/el pato/las_acacias_U5/</t>
+  </si>
+  <si>
+    <t>img1:/assets/images/properties/berazategui/el pato/las_acacias_U5/las_acacias_U5_1-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img2:las_acacias_U5_1-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img3:las_acacias_U5_1-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img4:las_acacias_U5_1-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img5:las_acacias_U5_10-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img6:las_acacias_U5_10-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img7:las_acacias_U5_10-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img8:las_acacias_U5_10-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img9:las_acacias_U5_11-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img10:las_acacias_U5_11-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img11:las_acacias_U5_11-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img12:las_acacias_U5_11-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img13:las_acacias_U5_12-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img14:las_acacias_U5_12-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img15:las_acacias_U5_12-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img16:las_acacias_U5_12-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img17:las_acacias_U5_2-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img18:las_acacias_U5_2-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img19:las_acacias_U5_2-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img20:las_acacias_U5_2-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img21:las_acacias_U5_3-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img22:las_acacias_U5_3-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img23:las_acacias_U5_3-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img24:las_acacias_U5_3-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img25:las_acacias_U5_4-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img26:las_acacias_U5_4-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img27:las_acacias_U5_4-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img28:las_acacias_U5_4-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img29:las_acacias_U5_5-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img30:las_acacias_U5_5-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img31:las_acacias_U5_5-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img32:las_acacias_U5_5-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img33:las_acacias_U5_6-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img34:las_acacias_U5_6-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img35:las_acacias_U5_6-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img36:las_acacias_U5_6-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img37:las_acacias_U5_7-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img38:las_acacias_U5_7-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img39:las_acacias_U5_7-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img40:las_acacias_U5_7-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img41:las_acacias_U5_8-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img42:las_acacias_U5_8-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img43:las_acacias_U5_8-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img44:las_acacias_U5_8-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img45:las_acacias_U5_9-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img46:las_acacias_U5_9-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img47:las_acacias_U5_9-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img48:las_acacias_U5_9-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img49:las_acacias_U5_1-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img50:las_acacias_U5_1-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img51:las_acacias_U5_1-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img52:las_acacias_U5_1-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img53:las_acacias_U5_10-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img54:las_acacias_U5_10-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img55:las_acacias_U5_10-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img56:las_acacias_U5_10-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img57:las_acacias_U5_11-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img58:las_acacias_U5_11-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img59:las_acacias_U5_11-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img60:las_acacias_U5_11-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img61:las_acacias_U5_12-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img62:las_acacias_U5_12-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img63:las_acacias_U5_12-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img64:las_acacias_U5_12-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img65:las_acacias_U5_2-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img66:las_acacias_U5_2-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img67:las_acacias_U5_2-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img68:las_acacias_U5_2-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img69:las_acacias_U5_3-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img70:las_acacias_U5_3-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img71:las_acacias_U5_3-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img72:las_acacias_U5_3-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img73:las_acacias_U5_4-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img74:las_acacias_U5_4-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img75:las_acacias_U5_4-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img76:las_acacias_U5_4-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img77:las_acacias_U5_5-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img78:las_acacias_U5_5-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img79:las_acacias_U5_5-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img80:las_acacias_U5_5-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img81:las_acacias_U5_6-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img82:las_acacias_U5_6-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img83:las_acacias_U5_6-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img84:las_acacias_U5_6-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img85:las_acacias_U5_7-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img86:las_acacias_U5_7-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img87:las_acacias_U5_7-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img88:las_acacias_U5_7-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img89:las_acacias_U5_8-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img90:las_acacias_U5_8-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img91:las_acacias_U5_8-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img92:las_acacias_U5_8-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img93:las_acacias_U5_9-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img94:las_acacias_U5_9-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img95:las_acacias_U5_9-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img96:las_acacias_U5_9-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/el pato/las_acacias_U5/las_acacias_U5_1-1024.webp</t>
   </si>
 </sst>
 </file>
@@ -981,19 +1011,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="45.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,52 +1031,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -1054,48 +1087,51 @@
         <f>CONCATENATE("/",A2,".html")</f>
         <v>/casa-gaboto5-hudson.html</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>220000</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>3</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>2</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1103,51 +1139,54 @@
         <f t="shared" ref="B3:B13" si="0">CONCATENATE("/",A3,".html")</f>
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>6000</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
       <c r="M3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1155,51 +1194,54 @@
         <f t="shared" si="0"/>
         <v>/loteo-aromas-laplata.html</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>8000</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="5"/>
+      <c r="R4" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1207,50 +1249,53 @@
         <f t="shared" si="0"/>
         <v>/loteo-elangel-laplata.html</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>12000</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1258,51 +1303,52 @@
         <f t="shared" si="0"/>
         <v>/loteo-bellavista-laplata.html</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>8000</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" t="s">
+      <c r="Q6" s="6"/>
+      <c r="R6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1310,51 +1356,52 @@
         <f t="shared" si="0"/>
         <v>/loteo-eleden-laplata.html</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>6000</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" t="s">
+      <c r="Q7" s="6"/>
+      <c r="R7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1362,48 +1409,49 @@
         <f t="shared" si="0"/>
         <v>/loteo-laspalmeras-laplata.html</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>10000</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1411,51 +1459,54 @@
         <f t="shared" si="0"/>
         <v>/loteo-nuevohorizone-laplata.html</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>23000</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>56</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" t="s">
+      <c r="Q9" s="6"/>
+      <c r="R9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1463,51 +1514,54 @@
         <f t="shared" si="0"/>
         <v>/loteo-santateresita-laplata.html</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>11000</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="6"/>
-      <c r="Q10" t="s">
+      <c r="Q10" s="6"/>
+      <c r="R10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1515,48 +1569,51 @@
         <f t="shared" si="0"/>
         <v>/casa-reta-tresarroyos.html</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>55000</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>3</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1564,119 +1621,132 @@
         <f t="shared" si="0"/>
         <v>/lotes-corderas-sanluis.html</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>8000</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>52</v>
       </c>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-venta-las-acacias.html</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="J13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="L13">
+        <v>55000</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
+      <c r="P13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="K13">
-        <v>55000</v>
-      </c>
-      <c r="L13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="R3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
hice cambios en el template
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D983CB-AB4C-4227-9788-7D38874B778A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451423E3-9498-4C15-9C20-F73C46B619DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18630" yWindow="1425" windowWidth="15300" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
   <si>
     <t>detailsPage</t>
-  </si>
-  <si>
-    <t>cover</t>
-  </si>
-  <si>
-    <t>images</t>
   </si>
   <si>
     <t>operation</t>
@@ -348,178 +342,6 @@
 Matias Settecerze CMYCP. 1219</t>
   </si>
   <si>
-    <t>/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/laspalmeras/laspalmeras-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/florenciovarela/laflorida/laflorida1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/aromas/aromas-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/elangel/elangel-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/bellavista/bellavista-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/eleden/eleden-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/tresarroyos/cabanareta/cabanareta-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/sanluis/corderas/corderas-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/santateresita/santateresita-1.webp</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/laplata/nuevohorizonte/nuevohorizonte-1.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-1.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img2:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-2.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img3:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-3.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img4:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-4.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img5:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-5.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img6:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-6.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img7:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-7.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img8:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-8.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img9:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-9.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img10:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-10.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img11:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-11.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img12:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-12.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img13:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-13.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img14:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-14.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img15:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-15.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img16:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-16.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img17:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-17.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img18:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-18.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img19:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-19.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto;
-img20:/assets/images/properties/berazategui/sebastiangaboto/5/gaboto5-20.webp,alt:Imágenes de casa en venta en Barrio Cerrado Sebastián Gaboto
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/florenciovarela/laflorida/laflorida1.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img2:/assets/images/properties/florenciovarela/laflorida/laflorida2.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img3:/assets/images/properties/florenciovarela/laflorida/laflorida3.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img4:/assets/images/properties/florenciovarela/laflorida/laflorida4.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img5:/assets/images/properties/florenciovarela/laflorida/laflorida5.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img6:/assets/images/properties/florenciovarela/laflorida/laflorida6.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img7:/assets/images/properties/florenciovarela/laflorida/laflorida7.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img8:/assets/images/properties/florenciovarela/laflorida/laflorida8.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img9:/assets/images/properties/florenciovarela/laflorida/laflorida9.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela;
-img10:/assets/images/properties/florenciovarela/laflorida/laflorida10.webp,alt:Imágenes de lotes en barrio abierto La Florida en Florencio Varela
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/aromas/aromas-1.webp,alt:Imágenes de lotes en Barrio Abierto Aromas en La Plata;
-img2:/assets/images/properties/laplata/aromas/aromas-2.webp,alt:Imágenes de lotes en Barrio Abierto Aromas en La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/elangel/elangel-1.webp,alt:Imágenes de lotes en Barrio Abierto El Ángel La Plata;
-img2:/assets/images/properties/laplata/elangel/elangel-2.webp,alt:Imágenes de lotes en Barrio Abierto El Ángel La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/bellavista/bellavista-1.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img2:/assets/images/properties/laplata/bellavista/bellavista-2.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img3:/assets/images/properties/laplata/bellavista/bellavista-3.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img4:/assets/images/properties/laplata/bellavista/bellavista-4.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img5:/assets/images/properties/laplata/bellavista/bellavista-5.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img6:/assets/images/properties/laplata/bellavista/bellavista-6.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img7:/assets/images/properties/laplata/bellavista/bellavista-7.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata;
-img8:/assets/images/properties/laplata/bellavista/bellavista-8.webp,alt:Imágenes de lotes en Barrio Abierto Bella Vista en La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/eleden/eleden-1.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img2:/assets/images/properties/laplata/eleden/eleden-2.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img3:/assets/images/properties/laplata/eleden/eleden-3.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img4:/assets/images/properties/laplata/eleden/eleden-4.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img5:/assets/images/properties/laplata/eleden/eleden-5.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img6:/assets/images/properties/laplata/eleden/eleden-6.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img7:/assets/images/properties/laplata/eleden/eleden-7.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata;
-img8:/assets/images/properties/laplata/eleden/eleden-8.webp,alt:Imágenes de lotes en Barrio Abierto El Edén en La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/laspalmeras/laspalmeras-1.webp,alt:Imágenes de lotes en Barrio Abierto Las Palmeras La Plata;
-img2:/assets/images/properties/laplata/laspalmeras/laspalmeras-2.webp,alt:Imágenes de lotes en Barrio Abierto Las Palmeras La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/nuevohorizonte/nuevohorizonte-1.webp,alt:Imágenes de lotes en Barrio Abierto Nuevo Horizonte La Plata;
-img2:/assets/images/properties/laplata/nuevohorizonte/nuevohorizonte-2.webp,alt:Imágenes de lotes en Barrio Abierto Nuevo Horizonte La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/laplata/santateresita/santateresita-1,alt:Imágenes de lotes en Barrio Abierto Santa Teresita La Plata;
-img2:/assets/images/properties/laplata/santateresita/santateresita-2,alt:Imágenes de lotes en Barrio Abierto Santa Teresita La Plata
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/tresarroyos/cabanareta/cabanareta-1.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img2:/assets/images/properties/tresarroyos/cabanareta/cabanareta-2.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img3:/assets/images/properties/tresarroyos/cabanareta/cabanareta-3.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img4:/assets/images/properties/tresarroyos/cabanareta/cabanareta-4.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img5:/assets/images/properties/tresarroyos/cabanareta/cabanareta-5.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img6:/assets/images/properties/tresarroyos/cabanareta/cabanareta-6.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img7:/assets/images/properties/tresarroyos/cabanareta/cabanareta-7.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img8:/assets/images/properties/tresarroyos/cabanareta/cabanareta-8.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img9:/assets/images/properties/tresarroyos/cabanareta/cabanareta-9.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img10:/assets/images/properties/tresarroyos/cabanareta/cabanareta-10.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img11:/assets/images/properties/tresarroyos/cabanareta/cabanareta-11.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img12:/assets/images/properties/tresarroyos/cabanareta/cabanareta-12.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img13:/assets/images/properties/tresarroyos/cabanareta/cabanareta-13.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img14:/assets/images/properties/tresarroyos/cabanareta/cabanareta-14.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img15:/assets/images/properties/tresarroyos/cabanareta/cabanareta-15.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img16:/assets/images/properties/tresarroyos/cabanareta/cabanareta-16.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img17:/assets/images/properties/tresarroyos/cabanareta/cabanareta-17.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img18:/assets/images/properties/tresarroyos/cabanareta/cabanareta-18.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img19:/assets/images/properties/tresarroyos/cabanareta/cabanareta-19.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img20:/assets/images/properties/tresarroyos/cabanareta/cabanareta-20.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img21:/assets/images/properties/tresarroyos/cabanareta/cabanareta-21.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img22:/assets/images/properties/tresarroyos/cabanareta/cabanareta-22.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img23:/assets/images/properties/tresarroyos/cabanareta/cabanareta-23.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img24:/assets/images/properties/tresarroyos/cabanareta/cabanareta-24.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos;
-img25:/assets/images/properties/tresarroyos/cabanareta/cabanareta-25.webp,alt:Imágenes de Cabaña en Reta Tres Arroyos
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img1:/assets/images/properties/sanluis/corderas/corderas-1.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img2:/assets/images/properties/sanluis/corderas/corderas-2.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img3:/assets/images/properties/sanluis/corderas/corderas-3.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img4:/assets/images/properties/sanluis/corderas/corderas-4.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img5:/assets/images/properties/sanluis/corderas/corderas-5.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img6:/assets/images/properties/sanluis/corderas/corderas-6.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img7:/assets/images/properties/sanluis/corderas/corderas-7.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img8:/assets/images/properties/sanluis/corderas/corderas-8.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img9:/assets/images/properties/sanluis/corderas/corderas-9.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img10:/assets/images/properties/sanluis/corderas/corderas-10.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img11:/assets/images/properties/sanluis/corderas/corderas-11.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img12:/assets/images/properties/sanluis/corderas/corderas-12.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img13:/assets/images/properties/sanluis/corderas/corderas-13.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img14:/assets/images/properties/sanluis/corderas/corderas-14.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img15:/assets/images/properties/sanluis/corderas/corderas-15.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img16:/assets/images/properties/sanluis/corderas/corderas-16.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img17:/assets/images/properties/sanluis/corderas/corderas-17.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img18:/assets/images/properties/sanluis/corderas/corderas-18.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img19:/assets/images/properties/sanluis/corderas/corderas-19.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img20:/assets/images/properties/sanluis/corderas/corderas-20.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img21:/assets/images/properties/sanluis/corderas/corderas-21.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img22:/assets/images/properties/sanluis/corderas/corderas-22.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img23:/assets/images/properties/sanluis/corderas/corderas-23.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img24:/assets/images/properties/sanluis/corderas/corderas-24.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis;
-img25:/assets/images/properties/sanluis/corderas/corderas-25.webp,alt:Imágenes de lotes en Barrio Abierto en Corderas San Luis
-</t>
-  </si>
-  <si>
     <t>video</t>
   </si>
   <si>
@@ -587,9 +409,6 @@
   </si>
   <si>
     <t>casa-venta-las-acacias</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1574.699881346684!2d-58.175552709271074!3d-34.88028292737519!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2d9ac6824eb15%3A0x65a407b05300e937!2sBarrio%20Las%20Acacias!5e0!3m2!1ses-419!2sar!4v1746032203480!5m2!1ses-419!2sar" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
   </si>
   <si>
     <t>El Pato, Berazategui</t>
@@ -647,13 +466,28 @@
     <t>/assets/images/properties/sanluis/corderas/</t>
   </si>
   <si>
-    <t>/assets/images/properties/berazategui/el pato/las_acacias_U5/</t>
-  </si>
-  <si>
-    <t>img1:/assets/images/properties/berazategui/el pato/las_acacias_U5/las_acacias_U5_1-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img2:las_acacias_U5_1-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img3:las_acacias_U5_1-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img4:las_acacias_U5_1-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img5:las_acacias_U5_10-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img6:las_acacias_U5_10-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img7:las_acacias_U5_10-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img8:las_acacias_U5_10-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img9:las_acacias_U5_11-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img10:las_acacias_U5_11-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img11:las_acacias_U5_11-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img12:las_acacias_U5_11-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img13:las_acacias_U5_12-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img14:las_acacias_U5_12-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img15:las_acacias_U5_12-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img16:las_acacias_U5_12-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img17:las_acacias_U5_2-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img18:las_acacias_U5_2-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img19:las_acacias_U5_2-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img20:las_acacias_U5_2-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img21:las_acacias_U5_3-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img22:las_acacias_U5_3-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img23:las_acacias_U5_3-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img24:las_acacias_U5_3-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img25:las_acacias_U5_4-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img26:las_acacias_U5_4-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img27:las_acacias_U5_4-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img28:las_acacias_U5_4-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img29:las_acacias_U5_5-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img30:las_acacias_U5_5-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img31:las_acacias_U5_5-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img32:las_acacias_U5_5-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img33:las_acacias_U5_6-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img34:las_acacias_U5_6-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img35:las_acacias_U5_6-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img36:las_acacias_U5_6-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img37:las_acacias_U5_7-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img38:las_acacias_U5_7-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img39:las_acacias_U5_7-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img40:las_acacias_U5_7-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img41:las_acacias_U5_8-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img42:las_acacias_U5_8-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img43:las_acacias_U5_8-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img44:las_acacias_U5_8-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img45:las_acacias_U5_9-1024.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img46:las_acacias_U5_9-1440.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img47:las_acacias_U5_9-480.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img48:las_acacias_U5_9-768.webp,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img49:las_acacias_U5_1-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img50:las_acacias_U5_1-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img51:las_acacias_U5_1-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img52:las_acacias_U5_1-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img53:las_acacias_U5_10-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img54:las_acacias_U5_10-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img55:las_acacias_U5_10-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img56:las_acacias_U5_10-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img57:las_acacias_U5_11-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img58:las_acacias_U5_11-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img59:las_acacias_U5_11-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img60:las_acacias_U5_11-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img61:las_acacias_U5_12-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img62:las_acacias_U5_12-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img63:las_acacias_U5_12-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img64:las_acacias_U5_12-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img65:las_acacias_U5_2-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img66:las_acacias_U5_2-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img67:las_acacias_U5_2-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img68:las_acacias_U5_2-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img69:las_acacias_U5_3-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img70:las_acacias_U5_3-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img71:las_acacias_U5_3-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img72:las_acacias_U5_3-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img73:las_acacias_U5_4-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img74:las_acacias_U5_4-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img75:las_acacias_U5_4-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img76:las_acacias_U5_4-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img77:las_acacias_U5_5-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img78:las_acacias_U5_5-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img79:las_acacias_U5_5-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img80:las_acacias_U5_5-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img81:las_acacias_U5_6-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img82:las_acacias_U5_6-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img83:las_acacias_U5_6-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img84:las_acacias_U5_6-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img85:las_acacias_U5_7-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img86:las_acacias_U5_7-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img87:las_acacias_U5_7-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img88:las_acacias_U5_7-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img89:las_acacias_U5_8-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img90:las_acacias_U5_8-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img91:las_acacias_U5_8-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img92:las_acacias_U5_8-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img93:las_acacias_U5_9-1024.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img94:las_acacias_U5_9-1440.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img95:las_acacias_U5_9-480.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;img96:las_acacias_U5_9-768.jpg,alt:Casa en venta en Barrio Cerrado Las Acacias, El Pato, Berazategui;</t>
-  </si>
-  <si>
-    <t>/assets/images/properties/berazategui/el pato/las_acacias_U5/las_acacias_U5_1-1024.webp</t>
+    <t>nombre_base_images</t>
+  </si>
+  <si>
+    <t>las_acacias_U5</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>Casa en venta en Barrio Cerrado Las Acacias</t>
+  </si>
+  <si>
+    <t>cantidad_imagenes</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m14!1m8!1m3!1d3273.061816595052!2d-58.17551100000001!3d-34.879794!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2d9ac6824eb15%3A0x65a407b05300e937!2sBarrio%20Las%20Acacias!5e0!3m2!1ses-419!2sar!4v1746459461600!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/el_pato/las_acacias_U5</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -1011,19 +845,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="45.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,700 +867,681 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="S1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>CONCATENATE("/",A2,".html")</f>
         <v>/casa-gaboto5-hudson.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="3">
+        <v>220000</v>
+      </c>
+      <c r="N2" s="2">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>55</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="3">
-        <v>220000</v>
-      </c>
-      <c r="M2" s="2">
-        <v>3</v>
-      </c>
-      <c r="N2" s="2">
-        <v>2</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="5"/>
-    </row>
-    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B13" si="0">CONCATENATE("/",A3,".html")</f>
+        <f t="shared" ref="B3:B12" si="0">CONCATENATE("/",A3,".html")</f>
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="3">
+        <v>6000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="3">
-        <v>6000</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="Q3" s="5"/>
-      <c r="R3" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="R3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-aromas-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4">
+        <v>8000</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4">
-        <v>8000</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="S4" s="5"/>
+      <c r="T4" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-elangel-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5">
         <v>12000</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="P5" t="s">
-        <v>65</v>
-      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="5"/>
       <c r="R5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="T5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-bellavista-laplata.html</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6">
         <v>8000</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q6" s="6"/>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="5"/>
       <c r="R6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="S6" s="6"/>
+      <c r="T6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-eleden-laplata.html</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="2" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7">
+        <v>14</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7">
         <v>6000</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="P7" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q7" s="6"/>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" s="5"/>
       <c r="R7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="S7" s="6"/>
+      <c r="T7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-laspalmeras-laplata.html</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="2" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8">
+        <v>14</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8">
         <v>10000</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
       <c r="N8">
         <v>0</v>
       </c>
-      <c r="O8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="P8" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-nuevohorizone-laplata.html</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="2" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9">
+        <v>14</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9">
         <v>23000</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q9" s="6"/>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="5"/>
       <c r="R9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-santateresita-laplata.html</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10">
+        <v>11000</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="6"/>
+      <c r="T10" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>41</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10">
-        <v>11000</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="P10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q10" s="6"/>
-      <c r="R10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-reta-tresarroyos.html</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" t="s">
-        <v>109</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>85</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11">
+        <v>55000</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L11">
-        <v>55000</v>
-      </c>
-      <c r="M11">
-        <v>3</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="5"/>
+      <c r="R11" t="s">
+        <v>49</v>
+      </c>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/lotes-corderas-sanluis.html</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12">
+        <v>8000</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" t="s">
+        <v>50</v>
+      </c>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>CONCATENATE("/",A13,".html")</f>
+        <v>/casa-venta-las-acacias.html</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="6">
+        <v>12</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12">
-        <v>8000</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="P12" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/casa-venta-las-acacias.html</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s">
-        <v>111</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L13">
+        <v>14</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13">
         <v>55000</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>3</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>1</v>
       </c>
-      <c r="O13" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
@@ -1746,7 +1563,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="T3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
cambie algunas cosas del home
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288E3FC4-C102-43E6-ADC6-6D6261305FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBF93FC-D818-4943-A484-C780526542B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="borrador" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -354,30 +355,6 @@
     <t>sqrmeters: - 300 m2; measurements: - medidas 13x23m; papers: -escritura y posesión inmediata; features: - cercano a escuelas y colectivos</t>
   </si>
   <si>
-    <t>pdf</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1ULWwQmBzbxELyJxhtQhCp0aDf8gE3JqF/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1q9kuPY7mAh3aTkQGNO2tCLvOSf3EnMf_/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1dAS5UNns9UX99WRzeMTZgDcLwcNGIG3z/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1jYMc9cz51lf8qFK42Md0q4os02Ymblu6/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1Nv3Wo__r0QIv_PMJFPH2CZ0ohgyevoGq/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1TTUdoRRzDyEri-U-tBw7ZUF5VmcjUN_g/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1iRYGPjeJOB-v8kLsc8QwlXbeuGojpHKu/view?usp=drive_link</t>
-  </si>
-  <si>
     <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m17!1m12!1m3!1d3275.2557002317585!2d-58.315628999999994!3d-34.824663!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m2!1m1!2zMzTCsDQ5JzI4LjgiUyA1OMKwMTgnNTYuMyJX!5e0!3m2!1ses-419!2sar!4v1740171257906!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
   </si>
   <si>
@@ -488,6 +465,45 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>gaboto_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casa en Venta en Barrio Cerrado Sebastian Gaboto Hudson Berazategui </t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/bellavista/</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/eleden/</t>
+  </si>
+  <si>
+    <t>cabana_reta</t>
+  </si>
+  <si>
+    <t>nuevos_horizonte</t>
+  </si>
+  <si>
+    <t>el_eden</t>
+  </si>
+  <si>
+    <t>bella_vista</t>
+  </si>
+  <si>
+    <t>la_florida</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en Fcio. Varela</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en Ruta 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lotes </t>
+  </si>
+  <si>
+    <t>250.000</t>
   </si>
 </sst>
 </file>
@@ -540,15 +556,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -564,6 +577,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -845,11 +865,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,6 +877,7 @@
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -867,16 +888,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -896,7 +917,7 @@
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -905,84 +926,549 @@
       <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="str">
+        <f t="shared" ref="B2:B8" si="0">CONCATENATE("/",A2,".html")</f>
+        <v>/casa-gaboto5-hudson.html</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="2">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/loteo-laflorida-fciovarela.html</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="9">
+        <v>6000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/loteo-bellavista-laplata.html</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="10">
+        <v>8000</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/loteo-eleden-laplata.html</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="10">
+        <v>6000</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/loteo-nuevohorizone-laplata.html</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="10">
+        <v>23000</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="4"/>
+      <c r="R6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/casa-reta-tresarroyos.html</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="10">
+        <v>55000</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" s="4"/>
+      <c r="R7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/casa-venta-las-acacias.html</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="5">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="10">
+        <v>55000</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B83F15-D7AB-43E8-94F1-997842D300EF}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="str">
+        <f>CONCATENATE("/",A1,".html")</f>
+        <v>/lotes-corderas-sanluis.html</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1">
+        <v>8000</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="4"/>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="str">
         <f>CONCATENATE("/",A2,".html")</f>
-        <v>/casa-gaboto5-hudson.html</v>
+        <v>/loteo-santateresita-laplata.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>89</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>66</v>
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="3">
-        <v>220000</v>
-      </c>
-      <c r="N2" s="2">
-        <v>3</v>
-      </c>
-      <c r="O2" s="2">
-        <v>2</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="M2">
+        <v>11000</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" t="s">
+        <v>52</v>
       </c>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
+    <row r="3" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B12" si="0">CONCATENATE("/",A3,".html")</f>
-        <v>/loteo-laflorida-fciovarela.html</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="5"/>
+        <f>CONCATENATE("/",A3,".html")</f>
+        <v>/loteo-laspalmeras-laplata.html</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="2" t="s">
@@ -991,60 +1477,57 @@
       <c r="H3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>76</v>
+      <c r="I3" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="3">
-        <v>6000</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
+      </c>
+      <c r="M3">
+        <v>10000</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" t="s">
+        <v>57</v>
       </c>
       <c r="S3" s="5"/>
-      <c r="T3" s="8" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-aromas-laplata.html</v>
+        <f>CONCATENATE("/",A4,".html")</f>
+        <v>/loteo-elangel-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>77</v>
+      <c r="I4" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>26</v>
@@ -1053,10 +1536,10 @@
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="M4">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1064,39 +1547,35 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="8" t="s">
-        <v>71</v>
+      <c r="P4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-elangel-laplata.html</v>
+        <f>CONCATENATE("/",A5,".html")</f>
+        <v>/loteo-aromas-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>78</v>
+      <c r="I5" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>26</v>
@@ -1105,10 +1584,10 @@
         <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M5">
-        <v>12000</v>
+        <v>8000</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1116,456 +1595,17 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-bellavista-laplata.html</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6">
-        <v>8000</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" t="s">
-        <v>61</v>
-      </c>
-      <c r="S6" s="6"/>
-      <c r="T6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-eleden-laplata.html</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7">
-        <v>6000</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7" s="6"/>
-      <c r="T7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-laspalmeras-laplata.html</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8">
-        <v>10000</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" t="s">
-        <v>57</v>
-      </c>
-      <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-nuevohorizone-laplata.html</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9">
-        <v>23000</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" t="s">
-        <v>54</v>
-      </c>
-      <c r="S9" s="6"/>
-      <c r="T9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/loteo-santateresita-laplata.html</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10">
-        <v>11000</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" t="s">
-        <v>52</v>
-      </c>
-      <c r="S10" s="6"/>
-      <c r="T10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/casa-reta-tresarroyos.html</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11">
-        <v>55000</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
-      </c>
-      <c r="O11">
-        <v>2</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" t="s">
-        <v>49</v>
-      </c>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>/lotes-corderas-sanluis.html</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M12">
-        <v>8000</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" t="s">
-        <v>50</v>
-      </c>
-      <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <f>CONCATENATE("/",A13,".html")</f>
-        <v>/casa-venta-las-acacias.html</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="6">
-        <v>12</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="s">
-        <v>105</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M13">
-        <v>55000</v>
-      </c>
-      <c r="N13">
-        <v>3</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="2:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="P5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="7"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="T3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregue fotos, faltan mas
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBF93FC-D818-4943-A484-C780526542B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B0C9DC-D582-49B2-A901-6C669CFD5224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="2010" windowWidth="15300" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
   <si>
     <t>id</t>
   </si>
@@ -114,23 +114,6 @@
     <t>Gaboto 5</t>
   </si>
   <si>
-    <t>¡Oportunidad única! Casa en construcción con entrega aproximada en junio 2025
-Ubicación: Sebastián Gaboto 05
-Superficie: 140 m² cubiertos + 45 m² semicubiertos + 42 m² solados
-- Vivienda en pozo en obra gris, se entrega con terminaciones de primera calidad:
-- Cielorrasos en yeso y hormigón visto en cocina-comedor
-- Pisos vinílicos SPC y porcelanato de alta gama
-- Pintura interior con látex mate + revestimiento exterior texturado
-- Parrilla con herraje regulable
-- Ventanas PVC con Doble Vidrio Hermético
-- Iluminación LED interna y externa
-- Cocina equipada con muebles completos y mesada de granito Negro Brasil
-- Baños con grifería FV y sanitarios Piazza
-Estado actual: Obra gris avanzada (platea, mampostería y losa listas)
-Consultanos para más info! ¡No dejes pasar esta oportunidad!
-Matias Settecerze CMYCP. 1219</t>
-  </si>
-  <si>
     <t>sqrmeters:🏠 140 m2 cubiertos; gallerysqrmeters:🏡 45 m2 semicubiertos; bedrooms:🛏️ 3 dormitorios; bathrooms:🚽 2 baños; livingroom:🛋️ Cocina, comedor y sala de estar, integrados; grill:👩‍🍳Galeria y parrilla; garage:🚘 Cochera</t>
   </si>
   <si>
@@ -504,6 +487,53 @@
   </si>
   <si>
     <t>250.000</t>
+  </si>
+  <si>
+    <t>Casa en Venta en B. Cerrado Sebastian Gaboto</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en La Plata Cce. Etcheverry</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en Florencio Varela</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en La Plata Ruta 36</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en La Plata Abasto</t>
+  </si>
+  <si>
+    <t>Cabaña en Reta, Tres Arroyos</t>
+  </si>
+  <si>
+    <t>¡Oportunidad única! Casa en construcción con entrega aproximada en junio 2025
+Ubicación: Sebastián Gaboto 05
+Superficie: 140 m² cubiertos + 45 m² semicubiertos + 42 m² solados
+- Vivienda en pozo en obra gris, se entrega con terminaciones de primera calidad:
+- Cielorrasos en yeso y hormigón visto en cocina-comedor
+- Pisos vinílicos SPC y porcelanato de alta gama
+- Pintura interior con látex mate + revestimiento exterior texturado
+- Parrilla con herraje regulable
+- Ventanas PVC con Doble Vidrio Hermético
+- Iluminación LED interna y externa
+- Cocina equipada con muebles completos y mesada de granito Negro Brasil
+- Baños con grifería FV y sanitarios Piazza
+Estado actual: Obra gris avanzada (platea, mampostería y losa listas)
+Consultanos para más info! ¡No dejes pasar esta oportunidad!
+Matias Settecerze CMYCP. 1219</t>
+  </si>
+  <si>
+    <t>6.000</t>
+  </si>
+  <si>
+    <t>55.000</t>
+  </si>
+  <si>
+    <t>8.000</t>
+  </si>
+  <si>
+    <t>23.000</t>
   </si>
 </sst>
 </file>
@@ -869,7 +899,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L3" sqref="L3"/>
+      <selection pane="topRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,16 +918,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -906,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -930,35 +960,35 @@
         <v>10</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B8" si="0">CONCATENATE("/",A2,".html")</f>
         <v>/casa-gaboto5-hudson.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="4">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
@@ -967,7 +997,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>21</v>
@@ -979,7 +1009,7 @@
         <v>22</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N2" s="2">
         <v>3</v>
@@ -988,15 +1018,17 @@
         <v>2</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="Q2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="R2" t="s">
+        <v>118</v>
+      </c>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1005,23 +1037,23 @@
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>16</v>
@@ -1032,8 +1064,8 @@
       <c r="L3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="9">
-        <v>6000</v>
+      <c r="M3" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -1044,8 +1076,10 @@
       <c r="P3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="S3" s="4"/>
@@ -1053,42 +1087,42 @@
     </row>
     <row r="4" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-bellavista-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="10">
-        <v>8000</v>
+        <v>29</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1097,50 +1131,54 @@
         <v>0</v>
       </c>
       <c r="P4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" t="s">
-        <v>61</v>
       </c>
       <c r="S4" s="5"/>
     </row>
     <row r="5" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-eleden-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="10">
-        <v>6000</v>
+        <v>41</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1149,27 +1187,29 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" t="s">
-        <v>59</v>
       </c>
       <c r="S5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-nuevohorizone-laplata.html</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -1177,22 +1217,22 @@
         <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="10">
-        <v>23000</v>
+        <v>43</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1201,27 +1241,29 @@
         <v>0</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" t="s">
         <v>54</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-reta-tresarroyos.html</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -1232,19 +1274,19 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="10">
-        <v>55000</v>
+        <v>45</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -1253,33 +1295,35 @@
         <v>2</v>
       </c>
       <c r="P7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="R7" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" t="s">
-        <v>49</v>
       </c>
       <c r="S7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-venta-las-acacias.html</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" s="5">
         <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
@@ -1288,19 +1332,19 @@
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M8" s="10">
-        <v>55000</v>
+        <v>79</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1309,13 +1353,13 @@
         <v>1</v>
       </c>
       <c r="P8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="R8" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1364,14 +1408,14 @@
   <sheetData>
     <row r="1" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>CONCATENATE("/",A1,".html")</f>
         <v>/lotes-corderas-sanluis.html</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1379,19 +1423,19 @@
         <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M1">
         <v>8000</v>
@@ -1403,24 +1447,24 @@
         <v>0</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>CONCATENATE("/",A2,".html")</f>
         <v>/loteo-santateresita-laplata.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -1428,19 +1472,19 @@
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M2">
         <v>11000</v>
@@ -1452,17 +1496,17 @@
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>CONCATENATE("/",A3,".html")</f>
@@ -1475,19 +1519,19 @@
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M3">
         <v>10000</v>
@@ -1499,24 +1543,24 @@
         <v>0</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>CONCATENATE("/",A4,".html")</f>
         <v>/loteo-elangel-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1524,19 +1568,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4">
         <v>12000</v>
@@ -1548,11 +1592,11 @@
         <v>0</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
@@ -1564,7 +1608,7 @@
         <v>/loteo-aromas-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1572,19 +1616,19 @@
         <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M5">
         <v>8000</v>
@@ -1596,11 +1640,11 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="7"/>

</xml_diff>

<commit_message>
arregle lo de los swipers. falta agregar fotos y datos
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B0C9DC-D582-49B2-A901-6C669CFD5224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C71815-92F7-4A57-990F-C39985609A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="2010" windowWidth="15300" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="135" windowWidth="19920" windowHeight="9375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -489,21 +489,6 @@
     <t>250.000</t>
   </si>
   <si>
-    <t>Casa en Venta en B. Cerrado Sebastian Gaboto</t>
-  </si>
-  <si>
-    <t>Lotes en Venta en La Plata Cce. Etcheverry</t>
-  </si>
-  <si>
-    <t>Lotes en Venta en Florencio Varela</t>
-  </si>
-  <si>
-    <t>Lotes en Venta en La Plata Ruta 36</t>
-  </si>
-  <si>
-    <t>Lotes en Venta en La Plata Abasto</t>
-  </si>
-  <si>
     <t>Cabaña en Reta, Tres Arroyos</t>
   </si>
   <si>
@@ -534,6 +519,24 @@
   </si>
   <si>
     <t>23.000</t>
+  </si>
+  <si>
+    <t>Casa en Barrio Cerrado Las Acacias</t>
+  </si>
+  <si>
+    <t>Lotes en La Plata Abasto</t>
+  </si>
+  <si>
+    <t>Lotes en La Plata Cce. Etcheverry</t>
+  </si>
+  <si>
+    <t>Lotes en La Plata Ruta 36</t>
+  </si>
+  <si>
+    <t>Lotes en Florencio Varela</t>
+  </si>
+  <si>
+    <t>Casa en B. Cerrado Sebastian Gaboto</t>
   </si>
 </sst>
 </file>
@@ -897,9 +900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P6" sqref="P6"/>
+      <selection pane="topRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,10 +1024,10 @@
         <v>23</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="R2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="S2" s="4"/>
     </row>
@@ -1065,7 +1068,7 @@
         <v>17</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -1077,7 +1080,7 @@
         <v>19</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>18</v>
@@ -1122,7 +1125,7 @@
         <v>29</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1134,7 +1137,7 @@
         <v>59</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>60</v>
@@ -1178,7 +1181,7 @@
         <v>41</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1190,7 +1193,7 @@
         <v>57</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>58</v>
@@ -1232,7 +1235,7 @@
         <v>43</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1244,7 +1247,7 @@
         <v>54</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>53</v>
@@ -1286,7 +1289,7 @@
         <v>45</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -1298,7 +1301,7 @@
         <v>47</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>48</v>
@@ -1344,7 +1347,7 @@
         <v>79</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1356,7 +1359,7 @@
         <v>80</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
termine de agregar fotos 1ra etapa
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C71815-92F7-4A57-990F-C39985609A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F289867-0984-46BE-8179-A83FE3BD511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="135" windowWidth="19920" windowHeight="9375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="141">
   <si>
     <t>id</t>
   </si>
@@ -402,9 +402,6 @@
     <t>folder</t>
   </si>
   <si>
-    <t>/assets/images/properties/berazategui/sebastiangaboto/5/</t>
-  </si>
-  <si>
     <t>/assets/images/properties/florenciovarela/laflorida</t>
   </si>
   <si>
@@ -463,9 +460,6 @@
   </si>
   <si>
     <t>cabana_reta</t>
-  </si>
-  <si>
-    <t>nuevos_horizonte</t>
   </si>
   <si>
     <t>el_eden</t>
@@ -537,6 +531,67 @@
   </si>
   <si>
     <t>Casa en B. Cerrado Sebastian Gaboto</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/sebastiangaboto/5</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/K4UO0jcoSRk?si=JXf5v_za3AM0l2xA</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/9rE2JP0Ipy4?feature=share</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/63zIMmqjpEM?feature=share</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/pDfS0O-Y98k?si=IcRhNjyEb3JsDmSE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/_YQzG2qIBH8?si=6bymA7-MW7Nbq0N4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/6A9nLeqCsiU</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/anaVxVbLYyM?si=JTVu6-eDkB0zQGIZ</t>
+  </si>
+  <si>
+    <t>lote_villa_elisa</t>
+  </si>
+  <si>
+    <t>lote-villa-elisa-calle-32</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en Barrio Abierto El Eden</t>
+  </si>
+  <si>
+    <t>Lotes en Venta en Barrio Abierto Nuevo Horizonte</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/XY1fZozjuQc?feature=share</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/laplata/villaelisa</t>
+  </si>
+  <si>
+    <t>Lote en Villa Elisa</t>
+  </si>
+  <si>
+    <t>48.000</t>
+  </si>
+  <si>
+    <t>sqrmeters:🌳 697 m2 cubiertos; measurements: 📏 medidas: 20x34,85m ; papers: 📝escritura; features: 🕊️ zona muy tranquila y privada</t>
+  </si>
+  <si>
+    <t>Lote en venta en Villa Elisa, partido de La Plata, con una superficie de casi 700 m². Ubicado en una zona residencial rodeada de quintas, ideal para quienes buscan naturaleza, espacio y tranquilidad sin alejarse de los accesos principales.
+La propiedad cuenta con una hermosa arboleda que aporta sombra, privacidad y un entorno natural único. El lote se encuentra a solo 500 metros de la estación de trenes Pereyra, a pocos minutos de la subida a la autopista Buenos Aires - La Plata y del centro de Villa Elisa, lo que brinda una excelente conectividad.
+Zona muy tranquila, con un entorno verde y cuidado. Ideal para vivienda permanente, casa de fin de semana o proyecto familiar.
+Documentación en regla, con escritura.
+Consultanos para más información o para coordinar una visita.</t>
+  </si>
+  <si>
+    <t>nuevo_horizonte</t>
   </si>
 </sst>
 </file>
@@ -589,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -617,6 +672,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -900,9 +958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3"/>
+      <selection pane="topRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,13 +982,13 @@
         <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -963,7 +1021,7 @@
         <v>10</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>11</v>
@@ -978,20 +1036,20 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f t="shared" ref="B2:B8" si="0">CONCATENATE("/",A2,".html")</f>
+        <f t="shared" ref="B2:B9" si="0">CONCATENATE("/",A2,".html")</f>
         <v>/casa-gaboto5-hudson.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="4">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
@@ -1012,7 +1070,7 @@
         <v>22</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N2" s="2">
         <v>3</v>
@@ -1024,14 +1082,16 @@
         <v>23</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R2" t="s">
-        <v>113</v>
-      </c>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1040,20 +1100,22 @@
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>105</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>67</v>
@@ -1068,7 +1130,7 @@
         <v>17</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -1080,12 +1142,14 @@
         <v>19</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="R3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="4"/>
+      <c r="S3" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1097,14 +1161,16 @@
         <v>/loteo-bellavista-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5</v>
+      </c>
       <c r="F4" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
@@ -1125,7 +1191,7 @@
         <v>29</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1137,12 +1203,14 @@
         <v>59</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="S4" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1153,15 +1221,17 @@
         <v>/loteo-eleden-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1181,7 +1251,7 @@
         <v>41</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1193,12 +1263,14 @@
         <v>57</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="S5" s="5"/>
+      <c r="S5" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1209,13 +1281,17 @@
         <v>/loteo-nuevohorizone-laplata.html</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1235,7 +1311,7 @@
         <v>43</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1247,12 +1323,14 @@
         <v>54</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="5"/>
+      <c r="S6" s="11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1263,13 +1341,17 @@
         <v>/casa-reta-tresarroyos.html</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="E7" s="5">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1289,7 +1371,7 @@
         <v>45</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -1301,12 +1383,14 @@
         <v>47</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="S7" s="5"/>
+      <c r="S7" s="11" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1317,16 +1401,16 @@
         <v>/casa-venta-las-acacias.html</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="5">
         <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
@@ -1335,7 +1419,7 @@
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>78</v>
@@ -1347,7 +1431,7 @@
         <v>79</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1359,15 +1443,62 @@
         <v>80</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="S8" s="7" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/lote-villa-elisa-calle-32.html</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="5">
+        <v>7</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="10" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -1394,8 +1525,18 @@
       <c r="C15" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S8" r:id="rId1" xr:uid="{171F0619-CBA6-420C-8593-336A4CD87F33}"/>
+    <hyperlink ref="S7" r:id="rId2" xr:uid="{B45C3F5B-0320-411A-9773-D272AAC58976}"/>
+    <hyperlink ref="S6" r:id="rId3" xr:uid="{F98107B1-67DD-46C7-975A-8F8C59DC6751}"/>
+    <hyperlink ref="S5" r:id="rId4" xr:uid="{FB25525C-EB4F-46A8-AAA9-5CE0D78BAD0F}"/>
+    <hyperlink ref="S4" r:id="rId5" xr:uid="{359EAFA4-62A7-4EDF-8002-506994070909}"/>
+    <hyperlink ref="S3" r:id="rId6" xr:uid="{63FDF07A-3E70-4C3E-9767-1BDD2FA6929A}"/>
+    <hyperlink ref="S2" r:id="rId7" xr:uid="{25FB0D48-F40B-4A28-A810-8B5DFB2CA14E}"/>
+    <hyperlink ref="S9" r:id="rId8" xr:uid="{EF652CF0-63C3-453D-84DD-4AED08780BDB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1418,7 +1559,7 @@
         <v>/lotes-corderas-sanluis.html</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1467,7 +1608,7 @@
         <v>/loteo-santateresita-laplata.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -1563,7 +1704,7 @@
         <v>/loteo-elangel-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1611,7 +1752,7 @@
         <v>/loteo-aromas-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>

</xml_diff>

<commit_message>
dejo todo guardado antes de seguir agregando mas propiedades
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F289867-0984-46BE-8179-A83FE3BD511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE67BDE-97DE-4D4F-832C-4E02E36DC846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="144">
   <si>
     <t>id</t>
   </si>
@@ -592,6 +592,15 @@
   </si>
   <si>
     <t>nuevo_horizonte</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m14!1m12!1m3!1d881.1099637930135!2d-58.08958720486494!3d-34.83991181994552!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!5e1!3m2!1ses-419!2sar!4v1747765908399!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Villa Elisa, La Plata</t>
+  </si>
+  <si>
+    <t>Calle 403 y 115 bis</t>
   </si>
 </sst>
 </file>
@@ -958,9 +967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +1486,18 @@
       </c>
       <c r="H9" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
guardo antes de probar galeria con tres swipers
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE67BDE-97DE-4D4F-832C-4E02E36DC846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26955B01-07C7-4426-BEEA-49AA5B6A6A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18645" yWindow="1155" windowWidth="15300" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="166">
   <si>
     <t>id</t>
   </si>
@@ -49,9 +49,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>rooms</t>
   </si>
   <si>
@@ -80,26 +77,6 @@
   </si>
   <si>
     <t>Amador Villa Abrille y Arroyo Las Piedras</t>
-  </si>
-  <si>
-    <t>¡Hacé realidad tu proyecto en el exclusivo barrio abierto La Florida en Florencio Varela! Una propuesta única diseñada para combinar naturaleza, comodidad y desarrollo.
-Características principales:
-Terrenos disponibles con posesión inmediata.
-Superficies aproximadas de 300 m², ideales para uso residencial o comercial.
-Espacios verdes: Contará con plazas y áreas de recreación, perfectas para disfrutar en familia.
-Un barrio exclusivo, pensado para el contacto con la naturaleza.
-Ubicación privilegiada:
-A 10 minutos del centro de Florencio Varela.
-Fácil acceso por Av. San Martín, Av. Sarmiento, y salida a la Av. Monteverde.
-A pocos minutos de la Unidad de Pronta Atención de Florencio Varela.
-Cercanía educativa: A 5 minutos de la Escuela Secundaria N°14 y el Colegio P. Mennel.
-Servicios y beneficios:
-Líneas 500 y 503 pasan a pocas cuadras.
-Próximo al Centro Deportivo La Patriada, el principal centro municipal de la zona.
-Lotes diseñados para uso comercial y residencial, adaptados a las necesidades de los habitantes.
-Opciones de financiación: ofrecemos planes de pago accesibles para que puedas adquirir tu lote sin complicaciones.
-No pierdas esta oportunidad de vivir o invertir en un entorno que lo tiene todo. ¡Consultanos hoy mismo y reservá tu lote!
-Matias Settecerze CMYCP. 1219</t>
   </si>
   <si>
     <t>sqrmeters: - 300 m2; type: - uso residencial o comecial; papers: -escritura y posesión inmediata; features: - cercano a escuelas y colectivos</t>
@@ -199,10 +176,6 @@
   </si>
   <si>
     <t>sqrmeters:🏠 64 m2 cubiertos; bedrooms:🛏️ 2 dormitorios; bathrooms:🚽 1 baño; livingroom:🛋️ Cocina, comedor y sala de estar, integrados; grill:👩‍🍳Galeria y parrilla; garage:🚘 Espacio guardacoche</t>
-  </si>
-  <si>
-    <t>Disfrutá de la tranquilidad de Reta en esta hermosa cabaña ubicada en Calle 15 entre 20 y 22, a solo dos cuadras del mar y con una vista privilegiada al océano. De acceso por arena, cuenta con un amplio espacio guarda coche para varios vehículos. En su interior, ofrece un ambiente cómodo y funcional con aire acondicionado, calefacción, dos dormitorios, un baño y un espacio integrado de living, cocina y comedor en planta baja. Además, dispone de lavadero, parrilla y un balcón ideal para relajarse. La propiedad cuenta con planos y escritura, brindando total seguridad jurídica. ¡No te pierdas esta oportunidad única de vivir cerca del mar!
-Matías Settecerze CMYCP. 1219</t>
   </si>
   <si>
     <t>Terrenos en venta en el valle de Cortaderas, con superficies de 990 a 1000 m² y hermosas vistas a la sierra. Ubicados a solo 20 cuadras de la Ruta 1 (Km 22) y a 15 minutos de la Villa de Merlo, con acceso rápido y seguro.
@@ -241,16 +214,6 @@
     <t>sqrmeters: - 497 m2; type: - uso residencial o comecial; papers: -escritura y posesión inmediata; features: - cercano a escuelas y colectivos</t>
   </si>
   <si>
-    <t>Ubicación: Calle 520 y 208, Abasto. A solo 200 metros de Av. 520, con acceso asfaltado.
-Superficie: 320 m² (12 metros de frente x 27 metros de fondo).
-Servicios: Lote con electricidad y demás servicios.
-Escritura individual y financiación disponible.
-Transporte: Líneas de colectivo cercanas: Oeste 14, Oeste 86 y 215B.
-Cercanías: A minutos del centro de salud (208 y 516 Bis) y del Jardín de Infantes N°930.
-Precios desde USD 23,000 a USD 35,000. Consultanos para más información.
-Matias Settecerze CMYCP. 1219</t>
-  </si>
-  <si>
     <t>sqrmeters: - 320 m2; measurements: - medidas: 12x27m ; papers: -escritura y posesión inmediata; features: - acceso de asfalto, lote con servicios</t>
   </si>
   <si>
@@ -274,38 +237,7 @@
     <t>sqrmeters: - 378 m2; measurements: - medidas: 12x31m ; papers: -escritura indivisa; features: -servicio de luz disponible</t>
   </si>
   <si>
-    <t>¡No te pierdas esta oportunidad única! El barrio abierto El Edén en Etcheverry, La Plata, ofrece los últimos lotes disponibles con excelentes características para vivir o invertir.
-Ubicación privilegiada:
-- A solo 1 cuadra de la Escuela N°61, que también incluye jardín y secundaria.
-- Próximo a la reconocida escuela La Sureña.
-- A pocos pasos de la plaza principal.
-- Cerca del Club Unión Vecinal A. Etcheverry.
-Acceso fácil y cómodo:
-- Ingreso pavimentado por Calle 52.
-- Parada final de los colectivos 11 y OE62 a pocos metros.
-Infraestructura y servicios:
-- Escritura indivisa: Tranquilidad legal garantizada.
-- Servicio de luz disponible en todos los terrenos.
-- Lotes amplios de 330 m² a 375 m².
-Opciones de financiación: ofrecemos planes de pago accesibles para que puedas adquirir tu lote sin complicaciones.
-¡Ideal para familias y proyectos personales! Contactanos para conocer más detalles y agendar una visita.
-Matias Settecerze CMYCP. 1219</t>
-  </si>
-  <si>
     <t>sqrmeters: - 300 m2; measurements: - medidas: 12x25m ; papers: -escritura indivisa; features: - accesos pavimentados y alumbrado público</t>
-  </si>
-  <si>
-    <t>Hacé realidad tu sueño de construir en el barrio abierto El Ángel, un lugar que lo tiene todo! Ideal para familias y proyectos personales, con una ubicación estratégica y servicios de calidad.
-Fácil acceso: Ubicado cerca de Av. 44 y Ruta 36.
-Zona con múltiples servicios y comercios para tu comodidad.
-Últimos lotes disponibles con escrituración y posesión inmediata.
-Accesos pavimentados y alumbrado público.
-Sobre calle asfaltada 203.
-Al lado del Parque Recreativo Los Olmos, un espacio perfecto para disfrutar al aire libre.
-A solo 1 cuadra del Club Peñarol, ideal para actividades deportivas y recreativas.
-Opciones de financiación. Planes accesibles para que puedas adquirir tu lote sin complicaciones.
-¡No te quedes afuera! Contactanos para más información y reservá tu lugar en El Ángel, donde todo está pensado para tu bienestar.
-Matias Settecerze CMYCP. 1219</t>
   </si>
   <si>
     <t>sqrmeters: - 300 m2; measurements: - medidas: 13x23m ; papers: -escritura indivisa; features: -  Fácil acceso a Av. 520 y Av. 44.</t>
@@ -380,25 +312,6 @@
     <t>sqrmeters:🏠 92 m2 cubiertos; bedrooms:🛏️ 3 dormitorios; bathrooms:🚽 1 baño; livingroom:🛋️ Cocina, comedor y sala de estar; garage:🚘 Cochera</t>
   </si>
   <si>
-    <t>Ubicada en un entorno tranquilo y organizado, esta propiedad cuenta con todo lo necesario para mudarse ya. Ideal para familias que buscan seguridad, comodidad y una excelente relación precio-calidad. Características principales:
--3 dormitorios
--Gran living-comedor
--Cocina independiente
--Hall de entrada
--Baño completo
--Lavadero
--Patio trasero
--Espacio para vehículo
-Entorno y servicios:
--Barrio cerrado con portón eléctrico
--Alarma vecinal
--Cámaras de seguridad
--Expensas muy bajas: menos de $5.000 por mes (incluyen corte de pasto de espacios comunes, uso de plaza interna y servicio de agua para el barrio)
--Plaza interna de uso común, ideal para niños o para disfrutar al aire libre.
-Accesos rápidos a la autopista y cercanía a comercios.
-Documentación al día – lista para escriturar.</t>
-  </si>
-  <si>
     <t>folder</t>
   </si>
   <si>
@@ -486,23 +399,6 @@
     <t>Cabaña en Reta, Tres Arroyos</t>
   </si>
   <si>
-    <t>¡Oportunidad única! Casa en construcción con entrega aproximada en junio 2025
-Ubicación: Sebastián Gaboto 05
-Superficie: 140 m² cubiertos + 45 m² semicubiertos + 42 m² solados
-- Vivienda en pozo en obra gris, se entrega con terminaciones de primera calidad:
-- Cielorrasos en yeso y hormigón visto en cocina-comedor
-- Pisos vinílicos SPC y porcelanato de alta gama
-- Pintura interior con látex mate + revestimiento exterior texturado
-- Parrilla con herraje regulable
-- Ventanas PVC con Doble Vidrio Hermético
-- Iluminación LED interna y externa
-- Cocina equipada con muebles completos y mesada de granito Negro Brasil
-- Baños con grifería FV y sanitarios Piazza
-Estado actual: Obra gris avanzada (platea, mampostería y losa listas)
-Consultanos para más info! ¡No dejes pasar esta oportunidad!
-Matias Settecerze CMYCP. 1219</t>
-  </si>
-  <si>
     <t>6.000</t>
   </si>
   <si>
@@ -584,13 +480,6 @@
     <t>sqrmeters:🌳 697 m2 cubiertos; measurements: 📏 medidas: 20x34,85m ; papers: 📝escritura; features: 🕊️ zona muy tranquila y privada</t>
   </si>
   <si>
-    <t>Lote en venta en Villa Elisa, partido de La Plata, con una superficie de casi 700 m². Ubicado en una zona residencial rodeada de quintas, ideal para quienes buscan naturaleza, espacio y tranquilidad sin alejarse de los accesos principales.
-La propiedad cuenta con una hermosa arboleda que aporta sombra, privacidad y un entorno natural único. El lote se encuentra a solo 500 metros de la estación de trenes Pereyra, a pocos minutos de la subida a la autopista Buenos Aires - La Plata y del centro de Villa Elisa, lo que brinda una excelente conectividad.
-Zona muy tranquila, con un entorno verde y cuidado. Ideal para vivienda permanente, casa de fin de semana o proyecto familiar.
-Documentación en regla, con escritura.
-Consultanos para más información o para coordinar una visita.</t>
-  </si>
-  <si>
     <t>nuevo_horizonte</t>
   </si>
   <si>
@@ -601,6 +490,242 @@
   </si>
   <si>
     <t>Calle 403 y 115 bis</t>
+  </si>
+  <si>
+    <t>nave-industrial-cir2-1300m2</t>
+  </si>
+  <si>
+    <t>nave-industrial-cir2-5800m2</t>
+  </si>
+  <si>
+    <t>nave-industrial-cir2-13800m2</t>
+  </si>
+  <si>
+    <t>/assets/images/properties/berazategui/el_pato/cir2</t>
+  </si>
+  <si>
+    <t>nave_ind_cir2_1300</t>
+  </si>
+  <si>
+    <t>nave_ind_cir2_5800</t>
+  </si>
+  <si>
+    <t>nave_ind_cir2_13800</t>
+  </si>
+  <si>
+    <t>Nave Industrial en Cir 2</t>
+  </si>
+  <si>
+    <t>Alquiler</t>
+  </si>
+  <si>
+    <t>Nave industrial</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3273.4417009125164!2d-58.17660787249145!3d-34.87025318192183!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2d8304ccb58c7%3A0x8bc0680e27601e90!2sParque%20industrial%20CIR2!5e0!3m2!1ses-419!2sar!4v1747770941967!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t> Au. 2 Colectora Este km 37.5</t>
+  </si>
+  <si>
+    <t>Nave Industrial de 1300m2 en Alquiler en Cir 2</t>
+  </si>
+  <si>
+    <t>Nave Industrial de 5800m2 en Alquiler en Cir 2</t>
+  </si>
+  <si>
+    <t>Nave Industrial de 13800m2 en Alquiler en Cir 2</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/QL_majT7DPY?feature=share</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/K5r8xMShgDg?feature=share</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/sAyULmch0Uc?feature=share</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;¡Hacé realidad tu proyecto en el exclusivo barrio abierto La Florida en Florencio Varela! Una propuesta única diseñada para combinar naturaleza, comodidad y desarrollo.&lt;br&gt;&lt;br&gt;
+Características principales:&lt;br&gt;&lt;br&gt;
+Terrenos disponibles con posesión inmediata.&lt;br&gt;
+Superficies aproximadas de 300 m², ideales para uso residencial o comercial.&lt;br&gt;
+Espacios verdes: Contará con plazas y áreas de recreación, perfectas para disfrutar en familia.&lt;br&gt;
+Un barrio exclusivo, pensado para el contacto con la naturaleza.&lt;br&gt;&lt;br&gt;
+Ubicación privilegiada:&lt;br&gt;&lt;br&gt;
+A 10 minutos del centro de Florencio Varela.&lt;br&gt;
+Fácil acceso por Av. San Martín, Av. Sarmiento, y salida a la Av. Monteverde.&lt;br&gt;
+A pocos minutos de la Unidad de Pronta Atención de Florencio Varela.&lt;br&gt;
+Cercanía educativa: A 5 minutos de la Escuela Secundaria N°14 y el Colegio P. Mennel.&lt;br&gt;&lt;br&gt;
+Servicios y beneficios:&lt;br&gt;&lt;br&gt;
+Líneas 500 y 503 pasan a pocas cuadras.&lt;br&gt;
+Próximo al Centro Deportivo La Patriada, el principal centro municipal de la zona.&lt;br&gt;
+Lotes diseñados para uso comercial y residencial, adaptados a las necesidades de los habitantes.&lt;br&gt;&lt;br&gt;
+Opciones de financiación: ofrecemos planes de pago accesibles para que puedas adquirir tu lote sin complicaciones.&lt;br&gt;&lt;br&gt;
+No pierdas esta oportunidad de vivir o invertir en un entorno que lo tiene todo. ¡Consultanos hoy mismo y reservá tu lote!&lt;br&gt;&lt;br&gt;
+Matias Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;¡Oportunidad única! Casa en construcción con entrega aproximada en junio 2025&lt;br&gt;Ubicación: Sebastián Gaboto 05&lt;br&gt;&lt;br&gt;
+Superficie: 140 m² cubiertos + 45 m² semicubiertos + 42 m² solados&lt;br&gt;
+- Vivienda en pozo en obra gris, se entrega con terminaciones de primera calidad:&lt;br&gt;
+- Cielorrasos en yeso y hormigón visto en cocina-comedor&lt;br&gt;
+- Pisos vinílicos SPC y porcelanato de alta gama&lt;br&gt;
+- Pintura interior con látex mate + revestimiento exterior texturado&lt;br&gt;
+- Parrilla con herraje regulable&lt;br&gt;
+- Ventanas PVC con Doble Vidrio Hermético&lt;br&gt;
+- Iluminación LED interna y externa&lt;br&gt;
+- Cocina equipada con muebles completos y mesada de granito Negro Brasil&lt;br&gt;
+- Baños con grifería FV y sanitarios Piazza&lt;br&gt;&lt;br&gt;
+Estado actual: Obra gris avanzada (platea, mampostería y losa listas)&lt;br&gt;&lt;br&gt;
+Consultanos para más info! ¡No dejes pasar esta oportunidad!&lt;br&gt;&lt;br&gt;
+Matias Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Hacé realidad tu sueño de construir en el barrio abierto El Ángel, un lugar que lo tiene todo! Ideal para familias y proyectos personales, con una ubicación estratégica y servicios de calidad.&lt;br&gt;&lt;br&gt;
+Fácil acceso: Ubicado cerca de Av. 44 y Ruta 36.&lt;br&gt;
+Zona con múltiples servicios y comercios para tu comodidad.&lt;br&gt;
+Últimos lotes disponibles con escrituración y posesión inmediata.&lt;br&gt;
+Accesos pavimentados y alumbrado público.&lt;br&gt;
+Sobre calle asfaltada 203.&lt;br&gt;
+Al lado del Parque Recreativo Los Olmos, un espacio perfecto para disfrutar al aire libre.&lt;br&gt;
+A solo 1 cuadra del Club Peñarol, ideal para actividades deportivas y recreativas.&lt;br&gt;&lt;br&gt;
+Opciones de financiación. Planes accesibles para que puedas adquirir tu lote sin complicaciones.&lt;br&gt;&lt;br&gt;
+¡No te quedes afuera! Contactanos para más información y reservá tu lugar en El Ángel, donde todo está pensado para tu bienestar.&lt;br&gt;&lt;br&gt;
+Matias Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;¡No te pierdas esta oportunidad única! El barrio abierto El Edén en Etcheverry, La Plata, ofrece los últimos lotes disponibles con excelentes características para vivir o invertir.&lt;br&gt;&lt;br&gt;
+Ubicación privilegiada:&lt;br&gt;
+- A solo 1 cuadra de la Escuela N°61, que también incluye jardín y secundaria.&lt;br&gt;
+- Próximo a la reconocida escuela La Sureña.&lt;br&gt;
+- A pocos pasos de la plaza principal.&lt;br&gt;
+- Cerca del Club Unión Vecinal A. Etcheverry.&lt;br&gt;&lt;br&gt;
+Acceso fácil y cómodo:&lt;br&gt;
+- Ingreso pavimentado por Calle 52.&lt;br&gt;
+- Parada final de los colectivos 11 y OE62 a pocos metros.&lt;br&gt;&lt;br&gt;
+Infraestructura y servicios:&lt;br&gt;
+- Escritura indivisa: Tranquilidad legal garantizada.&lt;br&gt;
+- Servicio de luz disponible en todos los terrenos.&lt;br&gt;
+- Lotes amplios de 330 m² a 375 m².&lt;br&gt;&lt;br&gt;
+Opciones de financiación: ofrecemos planes de pago accesibles para que puedas adquirir tu lote sin complicaciones.&lt;br&gt;&lt;br&gt;
+¡Ideal para familias y proyectos personales! Contactanos para conocer más detalles y agendar una visita.&lt;br&gt;&lt;br&gt;
+Matias Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Ubicación: Calle 520 y 208, Abasto. A solo 200 metros de Av. 520, con acceso asfaltado.&lt;br&gt;
+Superficie: 320 m² (12 metros de frente x 27 metros de fondo).&lt;br&gt;
+Servicios: Lote con electricidad y demás servicios.&lt;br&gt;
+Escritura individual y financiación disponible.&lt;br&gt;
+Transporte: Líneas de colectivo cercanas: Oeste 14, Oeste 86 y 215B.&lt;br&gt;
+Cercanías: A minutos del centro de salud (208 y 516 Bis) y del Jardín de Infantes N°930.&lt;br&gt;&lt;br&gt;
+Precios desde USD 23,000 a USD 35,000. Consultanos para más información.&lt;br&gt;&lt;br&gt;
+Matias Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Disfrutá de la tranquilidad de Reta en esta hermosa cabaña ubicada en Calle 15 entre 20 y 22, a solo dos cuadras del mar y con una vista privilegiada al océano. &lt;br&gt;&lt;br&gt;De acceso por arena, cuenta con un amplio espacio guarda coche para varios vehículos. En su interior, ofrece un ambiente cómodo y funcional con aire acondicionado, calefacción, dos dormitorios, un baño y un espacio integrado de living, cocina y comedor en planta baja. Además, dispone de lavadero, parrilla y un balcón ideal para relajarse.&lt;br&gt;&lt;br&gt; La propiedad cuenta con planos y escritura, brindando total seguridad jurídica. ¡No te pierdas esta oportunidad única de vivir cerca del mar!&lt;br&gt;&lt;br&gt;
+Matías Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Ubicada en un entorno tranquilo y organizado, esta propiedad cuenta con todo lo necesario para mudarse ya. Ideal para familias que buscan seguridad, comodidad y una excelente relación precio-calidad. Características principales:&lt;br&gt;
+-3 dormitorios&lt;br&gt;
+-Gran living-comedor&lt;br&gt;
+-Cocina independiente&lt;br&gt;
+-Hall de entrada&lt;br&gt;
+-Baño completo&lt;br&gt;
+-Lavadero&lt;br&gt;
+-Patio trasero&lt;br&gt;
+-Espacio para vehículo&lt;br&gt;&lt;br&gt;
+Entorno y servicios:&lt;br&gt;
+-Barrio cerrado con portón eléctrico&lt;br&gt;
+-Alarma vecinal&lt;br&gt;
+-Cámaras de seguridad&lt;br&gt;
+-Expensas muy bajas: menos de $5.000 por mes (incluyen corte de pasto de espacios comunes, uso de plaza interna y servicio de agua para el barrio)&lt;br&gt;
+-Plaza interna de uso común, ideal para niños o para disfrutar al aire libre.&lt;br&gt;&lt;br&gt;
+Accesos rápidos a la autopista y cercanía a comercios.&lt;br&gt;&lt;br&gt;
+Documentación al día – lista para escriturar.&lt;br&gt;&lt;br&gt;
+Matías Settecerze Col.1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Lote en venta en Villa Elisa, partido de La Plata, con una superficie de casi 700 m². Ubicado en una zona residencial rodeada de quintas, ideal para quienes buscan naturaleza, espacio y tranquilidad sin alejarse de los accesos principales.&lt;br&gt;&lt;br&gt;
+La propiedad cuenta con una hermosa arboleda que aporta sombra, privacidad y un entorno natural único. El lote se encuentra a solo 500 metros de la estación de trenes Pereyra, a pocos minutos de la subida a la autopista Buenos Aires - La Plata y del centro de Villa Elisa, lo que brinda una excelente conectividad.&lt;br&gt;&lt;br&gt;
+Zona muy tranquila, con un entorno verde y cuidado. Ideal para vivienda permanente, casa de fin de semana o proyecto familiar.&lt;br&gt;&lt;br&gt;
+Documentación en regla, con escritura.&lt;br&gt;&lt;br&gt;
+Consultanos para más información o para coordinar una visita.&lt;br&gt;&lt;br&gt; 
+Matías Settecerze Col.1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Alquiler Nave Industrial 5884 m² – Parque CIR2 El Pato – Amplia Nave + Oficinas&lt;br&gt;&lt;br&gt;
+Nave de 5.884,5 m² totales:&lt;br&gt;
+Galpón de 5.062,50 m²&lt;br&gt;
+Oficinas y baños: 822 m² (PB y PA)&lt;br&gt;&lt;br&gt;
+Dos portones de acceso para camiones .&lt;br&gt;
+Planta semi libre: columnas cada 7 m x 22 m&lt;br&gt;
+Techo tipo shed con gran ingreso de luz natural&lt;br&gt;
+Piso industrial de hormigón de alta resistencia&lt;br&gt;
+Ideal para logística, distribución o procesos productivos de gran escala.&lt;br&gt;&lt;br&gt;
+Parque Industrial CIR 2 – El Pato, Berazategui&lt;br&gt;
+Ubicado estratégicamente sobre la colectora de la Autovía 2, km 37½, entre Capital Federal y La Plata, con conexión directa a la Autopista Buenos Aires – La Plata. Cercano a los principales accesos terrestres, marítimos (Puerto de Buenos Aires) y aéreos (Ezeiza y Aeroparque).&lt;br&gt;&lt;br&gt;
+El predio cuenta con:&lt;br&gt;
+Seguridad 24 hs, red de cámaras y vigilancia interna y externa.&lt;br&gt;
+Energía eléctrica en media tensión, gas industrial, agua potable y planta de tratamiento de efluentes.&lt;br&gt;
+Cuartel de bomberos propio con autobomba, red hidrante y sistema antiincendio. &lt;br&gt;
+Oficinas, salas de reuniones, áreas de descanso, comedor, vestuarios y showroom.&lt;br&gt;
+Balanza electrónica de 80 tn, calles internas pavimentadas, y mantenimiento general continuo.&lt;br&gt;&lt;br&gt;
+Entorno ideal para logística, industria y operaciones con infraestructura de primer nivel.&lt;br&gt;&lt;br&gt;
+Consulte para más información. &lt;br&gt;&lt;br&gt;
+Matías Settecerze Col.1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Nave de 1.359 m² totales:&lt;br&gt;&lt;br&gt;
+Galpón de 1.181,50 m²&lt;br&gt;
+Oficinas y baños: 177,50 m²&lt;br&gt;&lt;br&gt;
+Acceso por portón apto para camión&lt;br&gt;
+Planta libre sin columnas, ideal para múltiples usos&lt;br&gt;
+Techo tipo shed con excelente ingreso de luz natural&lt;br&gt;
+Piso de hormigón de alta resistencia&lt;br&gt;
+Ideal para operaciones industriales, almacenamiento o logística de escala media.&lt;br&gt;&lt;br&gt;
+Parque Industrial CIR 2 – El Pato, Berazategui&lt;br&gt;&lt;br&gt;
+Ubicado estratégicamente sobre la colectora de la Autovía 2, km 37½, entre Capital Federal y La Plata, con conexión directa a la Autopista Buenos Aires – La Plata. Cercano a los principales accesos terrestres, marítimos (Puerto de Buenos Aires) y aéreos (Ezeiza y Aeroparque).&lt;br&gt;&lt;br&gt;
+El predio cuenta con:&lt;br&gt;
+Seguridad 24 hs, red de cámaras y vigilancia interna y externa.&lt;br&gt;
+Energía eléctrica en media tensión, gas industrial, agua potable y planta de tratamiento de efluentes.&lt;br&gt;
+Cuartel de bomberos propio con autobomba, red hidrante y sistema antiincendio.&lt;br&gt;
+Oficinas, salas de reuniones, áreas de descanso, comedor, vestuarios y showroom.&lt;br&gt;
+Balanza electrónica de 80 tn, calles internas pavimentadas, y mantenimiento general continuo.&lt;br&gt;&lt;br&gt;
+Entorno ideal para logística, industria y operaciones con infraestructura de primer nivel.&lt;br&gt;&lt;br&gt;
+Consulte para más información. &lt;br&gt;&lt;br&gt;
+Matías Settecerze Col.1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Nave de 13.835 m² totales:&lt;br&gt;
+Galpón de 13.170 m²&lt;br&gt;
+Oficinas y baños: 665 m²&lt;br&gt;&lt;br&gt;
+Varios ingresos para camiones de gran porte (5 m alto x 4 m ancho)&lt;br&gt;
+Planta semi libre (7 m entre columnas y 22 m entre líneas de columnas)&lt;br&gt;
+Altura a cabreada: 7 m&lt;br&gt;
+Techo tipo shed con luz natural&lt;br&gt;
+Detectores de humo recién instalados&lt;br&gt;
+Múltiples espacios de depósito&lt;br&gt;
+Piso de hormigón de alta resistencia&lt;br&gt;
+Ideal para industrias de gran volumen, centros logísticos o distribución nacional.&lt;br&gt;&lt;br&gt;
+Parque Industrial CIR 2 – El Pato, Berazategui&lt;br&gt;
+Ubicado estratégicamente sobre la colectora de la Autovía 2, km 37½, entre Capital Federal y La Plata, con conexión directa a la Autopista Buenos Aires – La Plata. Cercano a los principales accesos terrestres, marítimos (Puerto de Buenos Aires) y aéreos (Ezeiza y Aeroparque).&lt;br&gt;&lt;br&gt;
+El predio cuenta con:&lt;br&gt;
+Seguridad 24 hs, red de cámaras y vigilancia interna y externa.&lt;br&gt;
+Energía eléctrica en media tensión, gas industrial, agua potable y planta de tratamiento de efluentes.&lt;br&gt;
+Cuartel de bomberos propio con autobomba, red hidrante y sistema antiincendio. &lt;br&gt;
+Oficinas, salas de reuniones, áreas de descanso, comedor, vestuarios y showroom.&lt;br&gt;
+Balanza electrónica de 80 tn, calles internas pavimentadas, y mantenimiento general continuo.&lt;br&gt;&lt;br&gt;
+Entorno ideal para logística, industria y operaciones con infraestructura de primer nivel.&lt;br&gt;&lt;br&gt;
+Consulte para más información. &lt;br&gt;&lt;br&gt;
+Matías Settecerze Col.1219</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -967,9 +1092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,16 +1113,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1006,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -1018,68 +1143,68 @@
         <v>6</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f t="shared" ref="B2:B9" si="0">CONCATENATE("/",A2,".html")</f>
+        <f t="shared" ref="B2:B12" si="0">CONCATENATE("/",A2,".html")</f>
         <v>/casa-gaboto5-hudson.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E2" s="4">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="M2" s="9" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="N2" s="2">
         <v>3</v>
@@ -1088,58 +1213,58 @@
         <v>2</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" t="s">
+        <v>155</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="R2" t="s">
-        <v>111</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E3" s="4">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="M3" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -1148,59 +1273,59 @@
         <v>0</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="R3" t="s">
+        <v>154</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="R3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-bellavista-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1209,58 +1334,58 @@
         <v>0</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-eleden-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E5" s="5">
         <v>4</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1269,58 +1394,58 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-nuevohorizone-laplata.html</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E6" s="5">
         <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1329,58 +1454,58 @@
         <v>0</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S6" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-reta-tresarroyos.html</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E7" s="5">
         <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -1389,58 +1514,58 @@
         <v>2</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-venta-las-acacias.html</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E8" s="5">
         <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L8" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1449,58 +1574,58 @@
         <v>1</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/lote-villa-elisa-calle-32.html</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E9" s="5">
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" t="s">
-        <v>141</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L9" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1509,29 +1634,179 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/nave-industrial-cir2-1300m2.html</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" t="s">
+        <v>145</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="11" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/nave-industrial-cir2-5800m2.html</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="12" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/nave-industrial-cir2-13800m2.html</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="13" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -1555,9 +1830,12 @@
     <hyperlink ref="S3" r:id="rId6" xr:uid="{63FDF07A-3E70-4C3E-9767-1BDD2FA6929A}"/>
     <hyperlink ref="S2" r:id="rId7" xr:uid="{25FB0D48-F40B-4A28-A810-8B5DFB2CA14E}"/>
     <hyperlink ref="S9" r:id="rId8" xr:uid="{EF652CF0-63C3-453D-84DD-4AED08780BDB}"/>
+    <hyperlink ref="S12" r:id="rId9" xr:uid="{02E372F6-D5C2-450E-9107-6952A5D59297}"/>
+    <hyperlink ref="S10" r:id="rId10" xr:uid="{7A9C0442-8A4A-4AC4-9370-2868531F9055}"/>
+    <hyperlink ref="S11" r:id="rId11" xr:uid="{592EDC42-83C0-4C67-95D8-969C3C9CBA23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -1573,34 +1851,34 @@
   <sheetData>
     <row r="1" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>CONCATENATE("/",A1,".html")</f>
         <v>/lotes-corderas-sanluis.html</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M1">
         <v>8000</v>
@@ -1612,44 +1890,44 @@
         <v>0</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>CONCATENATE("/",A2,".html")</f>
         <v>/loteo-santateresita-laplata.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M2">
         <v>11000</v>
@@ -1661,17 +1939,17 @@
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>CONCATENATE("/",A3,".html")</f>
@@ -1681,22 +1959,22 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M3">
         <v>10000</v>
@@ -1708,44 +1986,44 @@
         <v>0</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>CONCATENATE("/",A4,".html")</f>
         <v>/loteo-elangel-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M4">
         <v>12000</v>
@@ -1757,43 +2035,43 @@
         <v>0</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>CONCATENATE("/",A5,".html")</f>
         <v>/loteo-aromas-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M5">
         <v>8000</v>
@@ -1805,11 +2083,11 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="7"/>

</xml_diff>

<commit_message>
agregue swipers diferentes segun tipo de propiedad. falta que ande bien el loop
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26955B01-07C7-4426-BEEA-49AA5B6A6A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548EB890-5F4E-4D85-9D39-04AFC12D3145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18645" yWindow="1155" windowWidth="15300" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18135" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>sqrmeters: - 300 m2; type: - uso residencial o comecial; papers: -escritura y posesión inmediata; features: - cercano a escuelas y colectivos</t>
   </si>
   <si>
-    <t>Casa</t>
-  </si>
-  <si>
     <t>Pueblos del Plata, Berazategui</t>
   </si>
   <si>
@@ -390,9 +387,6 @@
     <t>Lotes en Venta en Ruta 36</t>
   </si>
   <si>
-    <t xml:space="preserve">Lotes </t>
-  </si>
-  <si>
     <t>250.000</t>
   </si>
   <si>
@@ -514,12 +508,6 @@
   </si>
   <si>
     <t>Nave Industrial en Cir 2</t>
-  </si>
-  <si>
-    <t>Alquiler</t>
-  </si>
-  <si>
-    <t>Nave industrial</t>
   </si>
   <si>
     <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3273.4417009125164!2d-58.17660787249145!3d-34.87025318192183!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2d8304ccb58c7%3A0x8bc0680e27601e90!2sParque%20industrial%20CIR2!5e0!3m2!1ses-419!2sar!4v1747770941967!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
@@ -723,6 +711,18 @@
 Entorno ideal para logística, industria y operaciones con infraestructura de primer nivel.&lt;br&gt;&lt;br&gt;
 Consulte para más información. &lt;br&gt;&lt;br&gt;
 Matías Settecerze Col.1219</t>
+  </si>
+  <si>
+    <t>alquiler</t>
+  </si>
+  <si>
+    <t>lote</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>vivienda</t>
   </si>
   <si>
     <t>price</t>
@@ -1093,8 +1093,8 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P2" sqref="P2"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,16 +1113,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1131,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -1155,56 +1155,56 @@
         <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B12" si="0">CONCATENATE("/",A2,".html")</f>
         <v>/casa-gaboto5-hudson.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="4">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N2" s="2">
         <v>3</v>
@@ -1213,16 +1213,16 @@
         <v>2</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
@@ -1234,25 +1234,25 @@
         <v>/loteo-laflorida-fciovarela.html</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="4">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>101</v>
+        <v>162</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
@@ -1264,7 +1264,7 @@
         <v>16</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -1276,56 +1276,56 @@
         <v>17</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-bellavista-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1334,58 +1334,58 @@
         <v>0</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-eleden-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" s="5">
         <v>4</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1394,58 +1394,58 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/loteo-nuevohorizone-laplata.html</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" s="5">
         <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1454,58 +1454,58 @@
         <v>0</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-reta-tresarroyos.html</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="5">
         <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -1514,58 +1514,58 @@
         <v>2</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/casa-venta-las-acacias.html</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="5">
         <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1574,58 +1574,58 @@
         <v>1</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/lote-villa-elisa-calle-32.html</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="5">
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="I9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1634,55 +1634,55 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/nave-industrial-cir2-1300m2.html</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="I10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1691,52 +1691,52 @@
         <v>2</v>
       </c>
       <c r="Q10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="S10" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/nave-industrial-cir2-5800m2.html</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" t="s">
         <v>138</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="I11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N11">
         <v>5</v>
@@ -1745,52 +1745,52 @@
         <v>2</v>
       </c>
       <c r="Q11" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S11" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>/nave-industrial-cir2-13800m2.html</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" t="s">
         <v>141</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I12" t="s">
-        <v>145</v>
-      </c>
       <c r="J12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N12">
         <v>10</v>
@@ -1799,13 +1799,13 @@
         <v>4</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1851,14 +1851,14 @@
   <sheetData>
     <row r="1" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>CONCATENATE("/",A1,".html")</f>
         <v>/lotes-corderas-sanluis.html</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1866,19 +1866,19 @@
         <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M1">
         <v>8000</v>
@@ -1890,24 +1890,24 @@
         <v>0</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>CONCATENATE("/",A2,".html")</f>
         <v>/loteo-santateresita-laplata.html</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -1915,19 +1915,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M2">
         <v>11000</v>
@@ -1939,17 +1939,17 @@
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>CONCATENATE("/",A3,".html")</f>
@@ -1962,19 +1962,19 @@
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3">
         <v>10000</v>
@@ -1986,24 +1986,24 @@
         <v>0</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>CONCATENATE("/",A4,".html")</f>
         <v>/loteo-elangel-laplata.html</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2011,19 +2011,19 @@
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4">
         <v>12000</v>
@@ -2035,11 +2035,11 @@
         <v>0</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
@@ -2051,7 +2051,7 @@
         <v>/loteo-aromas-laplata.html</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2059,19 +2059,19 @@
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5">
         <v>8000</v>
@@ -2083,11 +2083,11 @@
         <v>0</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="7"/>

</xml_diff>

<commit_message>
agregue los dsan jose
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C07C83-4E18-443B-B3EC-7FB667836C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066DD892-7605-4203-861F-05455CDF2682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10200" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="243">
   <si>
     <t>id</t>
   </si>
@@ -784,9 +784,6 @@
     <t>lote_avingallan</t>
   </si>
   <si>
-    <t>lote_elpato_avingallan</t>
-  </si>
-  <si>
     <t>casa_elpato_508y621</t>
   </si>
   <si>
@@ -936,12 +933,150 @@
   <si>
     <t>feature1: 🏡 Cabaña rústica y tranquila; feature2: 🛏️ Dormitorio en entrepiso de madera; feature3: 🌳 Lote amplio con espacio libre; feature4: 📍 Acceso por calle de tierra en entorno natural</t>
   </si>
+  <si>
+    <t>lotes_elpato_avingallan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fs2WW2hqdpM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/j9o-Vpr1TW8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/LzBwgjNgW80</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/WCuU_URCXC4?si=E0dRD0Xc-2s3Mh2V</t>
+  </si>
+  <si>
+    <t>san_jose_II_30</t>
+  </si>
+  <si>
+    <t>san_jose_II_95</t>
+  </si>
+  <si>
+    <t>san_jose_IV_31y32</t>
+  </si>
+  <si>
+    <t>Lote en San José II</t>
+  </si>
+  <si>
+    <t>Lote con avances San José II</t>
+  </si>
+  <si>
+    <t>2 Lotes en San José IV</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3267.752017631686!2d-58.093724548446616!3d-35.01291228158296!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2c3003eca1779%3A0x34a505b8260106ff!2sBarrio%20cerrado%20San%20Jos%C3%A9%202!5e0!3m2!1ses-419!2sar!4v1748629769620!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3267.752017631686!2d-58.093724548446616!3d-35.01291228158296!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x95a2c3003a27194b%3A0x14ca8fb09f34db8!2sBarrio%20privado%20San%20Jose%20III-IV!5e0!3m2!1ses-419!2sar!4v1748629808373!5m2!1ses-419!2sar" width="100%" height="300" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Abasto, La Plata</t>
+  </si>
+  <si>
+    <t>San Clemente</t>
+  </si>
+  <si>
+    <t>C. 32 y 232</t>
+  </si>
+  <si>
+    <t>12.000</t>
+  </si>
+  <si>
+    <t>20.000</t>
+  </si>
+  <si>
+    <t>feature1: 📏 300 m² totales; feature2: 🌳 Cerca de la plaza central; feature3: ✅ Seguridad 24 hs; feature4: 🔑 Listo para escriturar con posesión inmediata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature1: 📏 300 m² totales; feature2: 🏗️ Futura casa de 3 dormitorios; feature3: ✅ Entradas y cerco perimetral; feature4: 🔑 Listo para escriturar </t>
+  </si>
+  <si>
+    <t>feature1: 🏞️ 2 lotes juntos (608 m²); feature2: 📐 Acceso desde 2 calles; feature3: 🌳 Barrio con seguridad 24 hs; feature4: 🔑 Listo para escriturar</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Lote en Venta en Barrio Cerrado San José II - Abasto&lt;br&gt;&lt;br&gt;
+Se vende lote en Barrio Cerrado San José II, ubicado en Calle 32, Abasto. Con una superficie de 300 m², este lote cuenta con orientación sur-oeste y se encuentra estratégicamente en diagonal a la plaza central, ofreciendo un entorno ideal para tu nuevo hogar o una quinta de descanso.&lt;br&gt;&lt;br&gt;
+Ubicación Estratégica:&lt;br&gt;
+A minutos de Ruta 2 con calles mejoradas.&lt;br&gt;
+Zona rodeada de barrios cerrados y quintas, perfecta para quienes buscan tranquilidad y contacto con la naturaleza.&lt;br&gt;&lt;br&gt;
+Servicios y Comodidades del Barrio:&lt;br&gt;
+Seguridad 24 hs con control de ingreso.&lt;br&gt;
+Cámaras de vigilancia y alarma vecinal.&lt;br&gt;
+Plaza con juegos infantiles y cancha de fútbol 5.&lt;br&gt;
+Mantenimiento de espacios comunes.&lt;br&gt;
+Agua corriente y tendido eléctrico listo para la bajada del medidor.&lt;br&gt;&lt;br&gt;
+Características del Lote:&lt;br&gt;
+Lote cercado en sus límites.&lt;br&gt;
+Listo para escriturar con posesión inmediata.&lt;br&gt;
+Expensas actuales: $55.000.&lt;br&gt;&lt;br&gt;
+Para más información o coordinar una visita, ¡no dudes en contactarnos! Estamos a tu disposición para ayudarte a encontrar tu próxima inversión.&lt;br&gt;&lt;br&gt; Matías Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Lote con Avance de Obra en Venta - Barrio Cerrado San José II&lt;br&gt;&lt;br&gt;
+Se vende lote con importante avance de obra en el Barrio Cerrado San José II, ubicado en Calle 32, Abasto. Con una superficie de 300 m², este terreno está preparado para construir la casa de tus sueños, con detalles que facilitan el inicio de tu proyecto.&lt;br&gt;&lt;br&gt;
+Ubicación Estratégica:&lt;br&gt;
+A minutos de Ruta 2 con calles mejoradas.&lt;br&gt;
+Zona rodeada de barrios cerrados y quintas, ideal para quienes buscan tranquilidad y contacto con la naturaleza.&lt;br&gt;&lt;br&gt;
+Servicios y Comodidades del Barrio:&lt;br&gt;
+Seguridad 24 hs con control de ingreso.&lt;br&gt;
+Cámaras de vigilancia y alarma vecinal.&lt;br&gt;
+Plaza con juegos infantiles y cancha de fútbol 5.&lt;br&gt;
+Mantenimiento de espacios comunes.&lt;br&gt;
+Agua corriente y tendido eléctrico listo para la bajada del medidor.&lt;br&gt;&lt;br&gt;
+Características Destacadas del Lote y Avance de Obra:&lt;br&gt;
+Entrada vehicular y peatonal de hormigón ya realizada.&lt;br&gt;
+Cerco perimetral completo.&lt;br&gt;
+Bases entoscadas y encadenado listo para la construcción de una casa con:&lt;br&gt;
+3 dormitorios&lt;br&gt;
+Living-comedor&lt;br&gt;
+Cocina&lt;br&gt;
+Baño principal y baño en suite&lt;br&gt;
+Despensa-lavadero&lt;br&gt;
+Pequeño patio libre al fondo y adelante&lt;br&gt;
+2 cocheras&lt;br&gt;&lt;br&gt;
+Listo para escriturar con posesión inmediata.&lt;br&gt;
+Expensas actuales: $55.000.&lt;br&gt;&lt;br&gt;
+No pierdas la oportunidad de tener tu casa en un barrio consolidado, con la ventaja de una obra ya iniciada. ¡Consultanos para más detalles y coordinar una visita!&lt;br&gt;&lt;br&gt; Matías Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Dos Lotes Juntos en Venta - Barrio Cerrado San José IV&lt;br&gt;&lt;br&gt;
+Se venden 2 lotes juntos en el exclusivo Barrio Cerrado San José IV, ubicado en Calle 32, Abasto. Con una superficie total de 608 m² y acceso desde dos calles, estos lotes ofrecen una gran versatilidad para diseñar una casa, una quinta de descanso o una vivienda permanente.&lt;br&gt;&lt;br&gt;
+Ubicación Estratégica:&lt;br&gt;
+A minutos de Ruta 2 con calles mejoradas.&lt;br&gt;
+Zona rodeada de barrios cerrados y quintas, ideal para quienes buscan tranquilidad y contacto con la naturaleza.&lt;br&gt;&lt;br&gt;
+Servicios y Comodidades del Barrio:&lt;br&gt;
+Seguridad 24 hs con control de ingreso.&lt;br&gt;
+Cámaras de vigilancia y alarma vecinal.&lt;br&gt;
+Laguna artificial y plaza privada.&lt;br&gt;
+Acceso a SUM (en construcción).&lt;br&gt;
+Agua corriente y tendido eléctrico listo para la bajada del medidor.&lt;br&gt;&lt;br&gt;
+Características de los Lotes:&lt;br&gt;
+Lotes amojonados, uno de sus laterales ya cercado.&lt;br&gt;
+Listos para escriturar con posesión inmediata.&lt;br&gt;
+Expensas actuales: $67.500 por lote.&lt;br&gt;&lt;br&gt;
+Para más información o coordinar una visita, contactanos. Estamos a tu disposición.&lt;br&gt;&lt;br&gt; Matías Settecerze Col. 1219</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/SBeWkRsWs-o?feature=share</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/zao_K_TZuT4?feature=share</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/BlSNloGd2wg?feature=share</t>
+  </si>
+  <si>
+    <t>https://youtube.com/embed/OJ2XmGrqx8M?si=g3LxOsDL11pod42O</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,6 +1096,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -987,7 +1130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1009,8 +1152,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1292,16 +1436,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M28" sqref="M27:M28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
@@ -1369,8 +1513,8 @@
       </c>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="4" t="str">
@@ -1380,13 +1524,13 @@
       <c r="C2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2">
         <v>7</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" t="s">
         <v>87</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1395,10 +1539,10 @@
       <c r="H2" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -1407,30 +1551,30 @@
       <c r="L2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2">
         <v>3</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2">
         <v>2</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="str">
@@ -1440,13 +1584,13 @@
       <c r="C3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" t="s">
         <v>94</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1455,10 +1599,10 @@
       <c r="H3" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -1467,30 +1611,30 @@
       <c r="L3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" t="s">
         <v>170</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" t="s">
         <v>106</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" t="s">
         <v>145</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="4" t="str">
@@ -1500,13 +1644,13 @@
       <c r="C4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" t="s">
         <v>95</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1515,10 +1659,10 @@
       <c r="H4" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -1527,30 +1671,30 @@
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" t="s">
         <v>171</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" t="s">
         <v>105</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" t="s">
         <v>147</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="4" t="str">
@@ -1560,13 +1704,13 @@
       <c r="C5" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" t="s">
         <v>118</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1575,10 +1719,10 @@
       <c r="H5" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -1587,30 +1731,30 @@
       <c r="L5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" t="s">
         <v>172</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="Q5" t="s">
         <v>104</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" t="s">
         <v>148</v>
       </c>
       <c r="S5" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="4" t="str">
@@ -1620,13 +1764,13 @@
       <c r="C6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" t="s">
         <v>119</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1635,10 +1779,10 @@
       <c r="H6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" t="s">
         <v>21</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1647,30 +1791,30 @@
       <c r="L6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" t="s">
         <v>173</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" t="s">
         <v>103</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" t="s">
         <v>149</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="4" t="str">
@@ -1680,13 +1824,13 @@
       <c r="C7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7">
         <v>14</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" t="s">
         <v>97</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1695,10 +1839,10 @@
       <c r="H7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" t="s">
         <v>32</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -1707,30 +1851,30 @@
       <c r="L7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7">
         <v>3</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" t="s">
         <v>97</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" t="s">
         <v>150</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="4" t="str">
@@ -1740,13 +1884,13 @@
       <c r="C8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8">
         <v>12</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" t="s">
         <v>81</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1755,10 +1899,10 @@
       <c r="H8" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" t="s">
         <v>67</v>
       </c>
       <c r="K8" s="4" t="s">
@@ -1767,30 +1911,30 @@
       <c r="L8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8">
         <v>3</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" t="s">
         <v>102</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="R8" t="s">
         <v>151</v>
       </c>
       <c r="S8" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="4" t="str">
@@ -1800,13 +1944,13 @@
       <c r="C9" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" t="s">
         <v>122</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1815,10 +1959,10 @@
       <c r="H9" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" t="s">
         <v>126</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" t="s">
         <v>127</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1827,30 +1971,30 @@
       <c r="L9" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" t="s">
         <v>124</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" t="s">
         <v>122</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" t="s">
         <v>152</v>
       </c>
       <c r="S9" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>129</v>
       </c>
       <c r="B10" s="4" t="str">
@@ -1860,13 +2004,13 @@
       <c r="C10" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10">
         <v>13</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" t="s">
         <v>135</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -1875,10 +2019,10 @@
       <c r="H10" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" t="s">
         <v>136</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="4" t="s">
@@ -1887,30 +2031,30 @@
       <c r="L10" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10">
         <v>1</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10">
         <v>2</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" t="s">
         <v>165</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" t="s">
         <v>139</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R10" t="s">
         <v>154</v>
       </c>
       <c r="S10" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>130</v>
       </c>
       <c r="B11" s="4" t="str">
@@ -1920,13 +2064,13 @@
       <c r="C11" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11">
         <v>7</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" t="s">
         <v>135</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1935,10 +2079,10 @@
       <c r="H11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" t="s">
         <v>136</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" t="s">
         <v>67</v>
       </c>
       <c r="K11" s="4" t="s">
@@ -1947,30 +2091,30 @@
       <c r="L11" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11">
         <v>5</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11">
         <v>2</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="P11" t="s">
         <v>166</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" t="s">
         <v>140</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="R11" t="s">
         <v>153</v>
       </c>
       <c r="S11" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>131</v>
       </c>
       <c r="B12" s="4" t="str">
@@ -1980,13 +2124,13 @@
       <c r="C12" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12">
         <v>8</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" t="s">
         <v>135</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -1995,10 +2139,10 @@
       <c r="H12" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" t="s">
         <v>136</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" t="s">
         <v>67</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -2007,30 +2151,30 @@
       <c r="L12" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12">
         <v>10</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12">
         <v>4</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="P12" t="s">
         <v>164</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="Q12" t="s">
         <v>141</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="R12" t="s">
         <v>155</v>
       </c>
       <c r="S12" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="str">
@@ -2040,13 +2184,13 @@
       <c r="C13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" t="s">
         <v>167</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13">
         <v>6</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" t="s">
         <v>168</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -2055,10 +2199,10 @@
       <c r="H13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" t="s">
         <v>21</v>
       </c>
       <c r="K13" s="4" t="s">
@@ -2067,45 +2211,46 @@
       <c r="L13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="N13" s="9">
+      <c r="M13" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="N13">
         <v>0</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="P13" t="s">
         <v>174</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="Q13" t="s">
         <v>168</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" t="s">
         <v>169</v>
       </c>
+      <c r="S13" s="9"/>
     </row>
-    <row r="14" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>175</v>
       </c>
       <c r="B14" s="4" t="str">
-        <f t="shared" ref="B14:B18" si="1">CONCATENATE("/",A14,".html")</f>
+        <f t="shared" ref="B14:B21" si="1">CONCATENATE("/",A14,".html")</f>
         <v>/cabana_512y624.html</v>
       </c>
       <c r="C14" s="4" t="str">
         <f xml:space="preserve"> CONCATENATE("/assets/images/properties/berazategui/el_pato/",A14,"/")</f>
         <v>/assets/images/properties/berazategui/el_pato/cabana_512y624/</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="D14" t="s">
+        <v>179</v>
+      </c>
+      <c r="E14">
         <v>12</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>186</v>
+      <c r="F14" t="s">
+        <v>185</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>12</v>
@@ -2113,36 +2258,42 @@
       <c r="H14" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I14" s="9" t="s">
-        <v>203</v>
+      <c r="I14" t="s">
+        <v>202</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="N14" s="9">
+        <v>207</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14">
         <v>1</v>
       </c>
-      <c r="P14" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="R14" s="9" t="s">
-        <v>199</v>
+      <c r="P14" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>185</v>
+      </c>
+      <c r="R14" t="s">
+        <v>198</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>176</v>
       </c>
       <c r="B15" s="4" t="str">
@@ -2153,14 +2304,14 @@
         <f xml:space="preserve"> CONCATENATE("/assets/images/properties/berazategui/el_pato/",A15,"/")</f>
         <v>/assets/images/properties/berazategui/el_pato/casa_508y621/</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15">
         <v>14</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>187</v>
+      <c r="F15" t="s">
+        <v>186</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>12</v>
@@ -2168,36 +2319,42 @@
       <c r="H15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>204</v>
+      <c r="I15" t="s">
+        <v>203</v>
+      </c>
+      <c r="J15" t="s">
+        <v>67</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="N15" s="9">
+        <v>205</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="N15">
         <v>4</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15">
         <v>2</v>
       </c>
-      <c r="P15" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q15" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="R15" s="9" t="s">
-        <v>198</v>
+      <c r="P15" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>186</v>
+      </c>
+      <c r="R15" t="s">
+        <v>197</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>177</v>
       </c>
       <c r="B16" s="4" t="str">
@@ -2208,14 +2365,14 @@
         <f xml:space="preserve"> CONCATENATE("/assets/images/properties/berazategui/el_pato/",A16,"/")</f>
         <v>/assets/images/properties/berazategui/el_pato/lote_avingallan/</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="D16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E16">
         <v>5</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>188</v>
+      <c r="F16" t="s">
+        <v>187</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>12</v>
@@ -2223,54 +2380,60 @@
       <c r="H16" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I16" s="9" t="s">
-        <v>200</v>
+      <c r="I16" t="s">
+        <v>199</v>
+      </c>
+      <c r="J16" t="s">
+        <v>67</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="N16" s="9">
+        <v>206</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="N16">
         <v>0</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="R16" s="9" t="s">
-        <v>197</v>
+      <c r="P16" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>187</v>
+      </c>
+      <c r="R16" t="s">
+        <v>196</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>181</v>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>180</v>
       </c>
       <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>/casa_peronyescalada.html</v>
       </c>
       <c r="C17" s="4" t="str">
-        <f xml:space="preserve"> CONCATENATE("/assets/images/properties/berazategui/el_pato/",A17,"/")</f>
-        <v>/assets/images/properties/berazategui/el_pato/casa_peronyescalada/</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E17" s="9">
+        <f xml:space="preserve"> CONCATENATE("/assets/images/properties/florenciovarela/casa_peronyescalada/")</f>
+        <v>/assets/images/properties/florenciovarela/casa_peronyescalada/</v>
+      </c>
+      <c r="D17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17">
         <v>7</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>189</v>
+      <c r="F17" t="s">
+        <v>188</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>12</v>
@@ -2278,53 +2441,59 @@
       <c r="H17" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>201</v>
+      <c r="I17" t="s">
+        <v>200</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="N17" s="9">
+        <v>204</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="N17">
         <v>6</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17">
         <v>3</v>
       </c>
-      <c r="P17" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="R17" s="9" t="s">
-        <v>210</v>
+      <c r="P17" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>188</v>
+      </c>
+      <c r="R17" t="s">
+        <v>209</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>184</v>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>183</v>
       </c>
       <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>/lote_avnaval.html</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E18" s="9">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18">
         <v>7</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>190</v>
+      <c r="F18" t="s">
+        <v>189</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>12</v>
@@ -2332,36 +2501,222 @@
       <c r="H18" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>202</v>
+      <c r="I18" t="s">
+        <v>201</v>
+      </c>
+      <c r="J18" t="s">
+        <v>229</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="N18" s="9">
+        <v>208</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="N18">
         <v>0</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q18" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="R18" s="9" t="s">
+      <c r="P18" t="s">
         <v>211</v>
       </c>
+      <c r="Q18" t="s">
+        <v>189</v>
+      </c>
+      <c r="R18" t="s">
+        <v>210</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="19" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M19" s="10"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>/san_jose_II_30.html</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f>CONCATENATE("/assets/images/properties/laplata/abasto/",A19)</f>
+        <v>/assets/images/properties/laplata/abasto/san_jose_II_30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" t="s">
+        <v>226</v>
+      </c>
+      <c r="J19" t="s">
+        <v>228</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>223</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>/san_jose_II_95.html</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f>CONCATENATE("/assets/images/properties/laplata/abasto/",A20)</f>
+        <v>/assets/images/properties/laplata/abasto/san_jose_II_95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>224</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" t="s">
+        <v>226</v>
+      </c>
+      <c r="J20" t="s">
+        <v>228</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>224</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>/san_jose_IV_31y32.html</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f>CONCATENATE("/assets/images/properties/laplata/abasto/",A21)</f>
+        <v>/assets/images/properties/laplata/abasto/san_jose_IV_31y32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>222</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I21" t="s">
+        <v>227</v>
+      </c>
+      <c r="J21" t="s">
+        <v>228</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>225</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="S21" s="11" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2376,9 +2731,17 @@
     <hyperlink ref="S6" r:id="rId9" xr:uid="{F98107B1-67DD-46C7-975A-8F8C59DC6751}"/>
     <hyperlink ref="S7" r:id="rId10" xr:uid="{B45C3F5B-0320-411A-9773-D272AAC58976}"/>
     <hyperlink ref="S8" r:id="rId11" xr:uid="{171F0619-CBA6-420C-8593-336A4CD87F33}"/>
+    <hyperlink ref="S16" r:id="rId12" xr:uid="{CE477509-0BB8-4A4A-9E89-1B760A04DD25}"/>
+    <hyperlink ref="S15" r:id="rId13" xr:uid="{44BBA9E1-50F5-4BF8-A9E8-1FF4EF787494}"/>
+    <hyperlink ref="S14" r:id="rId14" xr:uid="{559D94F2-5A4D-4AD7-B38F-00D2BD78AA68}"/>
+    <hyperlink ref="S18" r:id="rId15" xr:uid="{9D2DA58D-6B20-473A-8DE5-00E2AEE10EAB}"/>
+    <hyperlink ref="S17" r:id="rId16" xr:uid="{535BB926-E4A2-4AFA-BB45-E9D419F24E8B}"/>
+    <hyperlink ref="S20" r:id="rId17" xr:uid="{B2151961-CF71-4D5C-BCCE-307BAC3EFB0C}"/>
+    <hyperlink ref="S19" r:id="rId18" xr:uid="{DFDE7E94-53A4-45C8-B73A-2C72E83D3195}"/>
+    <hyperlink ref="S21" r:id="rId19" xr:uid="{24D3D055-0A66-44AC-8721-0E5E5EED4453}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sitio con admin uso
</commit_message>
<xml_diff>
--- a/assets/ddbb/properties.xlsx
+++ b/assets/ddbb/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DANI\msgrupoinmobiliario.com.ar\public_html\assets\ddbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066DD892-7605-4203-861F-05455CDF2682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70AA83C-DFD9-4EB4-9C99-0733793F8D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10200" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>48.000</t>
-  </si>
-  <si>
-    <t>sqrmeters:🌳 697 m2 cubiertos; measurements: 📏 medidas: 20x34,85m ; papers: 📝escritura; features: 🕊️ zona muy tranquila y privada</t>
   </si>
   <si>
     <t>nuevo_horizonte</t>
@@ -761,18 +758,6 @@
   </si>
   <si>
     <t>sqrmeters: 📐 300 m2; type: 🏡 uso residencial o comecial; papers: 📋 escritura y posesión inmediata; features: 🚌 cercano a escuelas y colectivos</t>
-  </si>
-  <si>
-    <t>sqrmeters: 📐 300 m2; measurements: medidas: 📏 12x25m ; papers: 📋 escritura indivisa; features: 🚗 accesos pavimentados y alumbrado público</t>
-  </si>
-  <si>
-    <t>sqrmeters: 📐 378 m2; measurements: 📏 medidas: 12x31m ; papers: 📋 escritura indivisa; features: ⚡ servicio de luz disponible</t>
-  </si>
-  <si>
-    <t>sqrmeters: 📐 320 m2; measurements: 📏 medidas: 12x27m ; papers: 📋 escritura y posesión inmediata; features: 🚗 acceso de asfalto</t>
-  </si>
-  <si>
-    <t>sqrmeters: 📐 300 m2; measurements: 📏 medidas: 13x23m ; papers: 📋 escritura indivisa; features: 📍  Fácil acceso a Av. 520 y Av. 44.</t>
   </si>
   <si>
     <t>cabana_512y624</t>
@@ -1070,6 +1055,21 @@
   </si>
   <si>
     <t>https://youtube.com/embed/OJ2XmGrqx8M?si=g3LxOsDL11pod42O</t>
+  </si>
+  <si>
+    <t>sqrmeters: 📐 320 m2; measurements: 📏 12x27m ; papers: 📋 escritura y posesión inmediata; features: 🚗 acceso de asfalto</t>
+  </si>
+  <si>
+    <t>sqrmeters: 📐 378 m2; measurements: 📏 12x31m ; papers: 📋 escritura indivisa; features: ⚡ servicio de luz disponible</t>
+  </si>
+  <si>
+    <t>sqrmeters: 📐 300 m2; measurements: 📏 12x25m ; papers: 📋 escritura indivisa; features: 🚗 accesos pavimentados y alumbrado público</t>
+  </si>
+  <si>
+    <t>sqrmeters:🌳 697 m2 cubiertos; measurements: 📏 20x34,85m ; papers: 📝escritura; features: 🕊️ zona muy tranquila y privada</t>
+  </si>
+  <si>
+    <t>sqrmeters: 📐 300 m2; measurements: 📏 13x23m ; papers: 📋 escritura indivisa; features: 📍  Fácil acceso a Av. 520 y Av. 44.</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1153,7 +1153,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1438,13 +1437,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
@@ -1491,7 +1491,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
@@ -1537,7 +1537,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I2" t="s">
         <v>54</v>
@@ -1567,7 +1567,7 @@
         <v>107</v>
       </c>
       <c r="R2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>115</v>
@@ -1597,7 +1597,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
         <v>56</v>
@@ -1621,13 +1621,13 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q3" t="s">
         <v>106</v>
       </c>
       <c r="R3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>114</v>
@@ -1657,7 +1657,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
         <v>59</v>
@@ -1681,13 +1681,13 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>171</v>
+        <v>240</v>
       </c>
       <c r="Q4" t="s">
         <v>105</v>
       </c>
       <c r="R4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>113</v>
@@ -1717,7 +1717,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -1741,13 +1741,13 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>172</v>
+        <v>239</v>
       </c>
       <c r="Q5" t="s">
         <v>104</v>
       </c>
       <c r="R5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S5" s="9" t="s">
         <v>112</v>
@@ -1765,7 +1765,7 @@
         <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1777,7 +1777,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
         <v>62</v>
@@ -1801,13 +1801,13 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
       <c r="Q6" t="s">
         <v>103</v>
       </c>
       <c r="R6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>111</v>
@@ -1837,7 +1837,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I7" t="s">
         <v>65</v>
@@ -1867,7 +1867,7 @@
         <v>97</v>
       </c>
       <c r="R7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>110</v>
@@ -1897,7 +1897,7 @@
         <v>12</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I8" t="s">
         <v>83</v>
@@ -1927,7 +1927,7 @@
         <v>102</v>
       </c>
       <c r="R8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S8" s="9" t="s">
         <v>109</v>
@@ -1957,19 +1957,19 @@
         <v>12</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" t="s">
         <v>126</v>
-      </c>
-      <c r="J9" t="s">
-        <v>127</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>123</v>
@@ -1981,13 +1981,13 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>124</v>
+        <v>241</v>
       </c>
       <c r="Q9" t="s">
         <v>122</v>
       </c>
       <c r="R9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S9" s="9" t="s">
         <v>120</v>
@@ -1995,32 +1995,32 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/nave-industrial-cir2-1300m2.html</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10">
         <v>13</v>
       </c>
       <c r="F10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" t="s">
         <v>135</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I10" t="s">
-        <v>136</v>
       </c>
       <c r="J10" t="s">
         <v>67</v>
@@ -2029,10 +2029,10 @@
         <v>13</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2041,46 +2041,46 @@
         <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/nave-industrial-cir2-5800m2.html</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11">
         <v>7</v>
       </c>
       <c r="F11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" t="s">
         <v>135</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I11" t="s">
-        <v>136</v>
       </c>
       <c r="J11" t="s">
         <v>67</v>
@@ -2089,10 +2089,10 @@
         <v>13</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N11">
         <v>5</v>
@@ -2101,46 +2101,46 @@
         <v>2</v>
       </c>
       <c r="P11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/nave-industrial-cir2-13800m2.html</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12">
         <v>8</v>
       </c>
       <c r="F12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12" t="s">
         <v>135</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I12" t="s">
-        <v>136</v>
       </c>
       <c r="J12" t="s">
         <v>67</v>
@@ -2149,10 +2149,10 @@
         <v>13</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N12">
         <v>10</v>
@@ -2161,16 +2161,16 @@
         <v>4</v>
       </c>
       <c r="P12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q12" t="s">
+        <v>140</v>
+      </c>
+      <c r="R12" t="s">
+        <v>154</v>
+      </c>
+      <c r="S12" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="R12" t="s">
-        <v>155</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -2185,19 +2185,19 @@
         <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E13">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I13" t="s">
         <v>58</v>
@@ -2212,7 +2212,7 @@
         <v>27</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2221,19 +2221,19 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="Q13" t="s">
+        <v>167</v>
+      </c>
+      <c r="R13" t="s">
         <v>168</v>
-      </c>
-      <c r="R13" t="s">
-        <v>169</v>
       </c>
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B14" s="4" t="str">
         <f t="shared" ref="B14:B21" si="1">CONCATENATE("/",A14,".html")</f>
@@ -2244,22 +2244,22 @@
         <v>/assets/images/properties/berazategui/el_pato/cabana_512y624/</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I14" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="J14" t="s">
         <v>67</v>
@@ -2268,10 +2268,10 @@
         <v>13</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2280,21 +2280,21 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="Q14" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="R14" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2305,22 +2305,22 @@
         <v>/assets/images/properties/berazategui/el_pato/casa_508y621/</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="J15" t="s">
         <v>67</v>
@@ -2329,10 +2329,10 @@
         <v>13</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="N15">
         <v>4</v>
@@ -2341,21 +2341,21 @@
         <v>2</v>
       </c>
       <c r="P15" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="Q15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="R15" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2366,22 +2366,22 @@
         <v>/assets/images/properties/berazategui/el_pato/lote_avingallan/</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E16">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I16" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="J16" t="s">
         <v>67</v>
@@ -2390,10 +2390,10 @@
         <v>13</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2402,21 +2402,21 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="Q16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="R16" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2427,22 +2427,22 @@
         <v>/assets/images/properties/florenciovarela/casa_peronyescalada/</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E17">
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I17" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="J17" t="s">
         <v>15</v>
@@ -2451,10 +2451,10 @@
         <v>13</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="N17">
         <v>6</v>
@@ -2463,58 +2463,58 @@
         <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="Q17" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="R17" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>/lote_avnaval.html</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E18">
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I18" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="J18" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2523,21 +2523,21 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="Q18" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="R18" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B19" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2548,34 +2548,34 @@
         <v>/assets/images/properties/laplata/abasto/san_jose_II_30</v>
       </c>
       <c r="D19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E19">
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I19" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J19" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -2584,21 +2584,21 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="Q19" t="s">
-        <v>223</v>
-      </c>
-      <c r="R19" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="R19" t="s">
+        <v>231</v>
+      </c>
+      <c r="S19" s="10" t="s">
         <v>236</v>
-      </c>
-      <c r="S19" s="11" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2609,34 +2609,34 @@
         <v>/assets/images/properties/laplata/abasto/san_jose_II_95</v>
       </c>
       <c r="D20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E20">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I20" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J20" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="N20">
         <v>3</v>
@@ -2645,21 +2645,21 @@
         <v>2</v>
       </c>
       <c r="P20" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="Q20" t="s">
-        <v>224</v>
-      </c>
-      <c r="R20" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="S20" s="11" t="s">
-        <v>240</v>
+        <v>219</v>
+      </c>
+      <c r="R20" t="s">
+        <v>232</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B21" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2670,34 +2670,34 @@
         <v>/assets/images/properties/laplata/abasto/san_jose_IV_31y32</v>
       </c>
       <c r="D21" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E21">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I21" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J21" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2706,16 +2706,16 @@
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="Q21" t="s">
-        <v>225</v>
-      </c>
-      <c r="R21" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="S21" s="11" t="s">
-        <v>242</v>
+        <v>220</v>
+      </c>
+      <c r="R21" t="s">
+        <v>233</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>